<commit_message>
post ops update 2020
</commit_message>
<xml_diff>
--- a/static/download/2020/RP3_ERT_ATFM_2020_Jan_Dec.xlsx
+++ b/static/download/2020/RP3_ERT_ATFM_2020_Jan_Dec.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="212" uniqueCount="158">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="214" uniqueCount="160">
   <si>
     <t>Data source</t>
   </si>
@@ -489,6 +489,12 @@
   </si>
   <si>
     <t>Comment</t>
+  </si>
+  <si>
+    <t>All</t>
+  </si>
+  <si>
+    <t>Data updated with post-ops adjustments</t>
   </si>
 </sst>
 </file>
@@ -843,7 +849,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="106">
+  <cellXfs count="107">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -1138,19 +1144,22 @@
       <alignment shrinkToFit="0" wrapText="0"/>
     </xf>
     <xf borderId="0" fillId="3" fontId="10" numFmtId="164" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
-      <alignment horizontal="center" shrinkToFit="0" vertical="bottom" wrapText="0"/>
+      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
     <xf borderId="0" fillId="3" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
     <xf borderId="0" fillId="3" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
+    </xf>
+    <xf borderId="0" fillId="3" fontId="10" numFmtId="164" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
+      <alignment horizontal="center" shrinkToFit="0" vertical="bottom" wrapText="0"/>
+    </xf>
+    <xf borderId="0" fillId="3" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="center" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="10" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0" shrinkToFit="0" wrapText="0"/>
-    </xf>
-    <xf borderId="0" fillId="3" fontId="10" numFmtId="164" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
-      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
     <xf borderId="0" fillId="3" fontId="6" numFmtId="17" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
       <alignment vertical="bottom"/>
@@ -1234,7 +1243,7 @@
         <v>4</v>
       </c>
       <c r="B2" s="10">
-        <v>44209.0</v>
+        <v>44308.0</v>
       </c>
       <c r="C2" s="11" t="s">
         <v>5</v>
@@ -1450,20 +1459,20 @@
       </c>
       <c r="C11" s="31">
         <f t="shared" si="1"/>
-        <v>0.3517423594</v>
+        <v>0.348000394</v>
       </c>
       <c r="D11" s="38">
         <v>4608808.0</v>
       </c>
       <c r="E11" s="39">
-        <v>1621113.0</v>
+        <v>1603867.0</v>
       </c>
       <c r="F11" s="42">
         <v>0.9</v>
       </c>
       <c r="G11" s="41">
         <f t="shared" si="2"/>
-        <v>-0.5482576406</v>
+        <v>-0.551999606</v>
       </c>
       <c r="H11" s="36">
         <v>0.0071</v>
@@ -1587,7 +1596,7 @@
         <v>4</v>
       </c>
       <c r="B2" s="10">
-        <v>44209.0</v>
+        <v>44308.0</v>
       </c>
       <c r="C2" s="11" t="s">
         <v>5</v>
@@ -1652,13 +1661,13 @@
       </c>
       <c r="B6" s="62">
         <f t="shared" ref="B6:B29" si="1">D6/C6</f>
-        <v>0.3901494621</v>
+        <v>0.3881771646</v>
       </c>
       <c r="C6" s="63">
         <v>730620.0</v>
       </c>
       <c r="D6" s="64">
-        <v>285051.0</v>
+        <v>283610.0</v>
       </c>
       <c r="E6" s="65"/>
       <c r="F6" s="66">
@@ -1671,13 +1680,13 @@
       </c>
       <c r="B7" s="67">
         <f t="shared" si="1"/>
-        <v>0.489219714</v>
+        <v>0.4865745041</v>
       </c>
       <c r="C7" s="68">
         <v>686902.0</v>
       </c>
       <c r="D7" s="69">
-        <v>336046.0</v>
+        <v>334229.0</v>
       </c>
       <c r="E7" s="65"/>
       <c r="F7" s="66">
@@ -1690,13 +1699,13 @@
       </c>
       <c r="B8" s="67">
         <f t="shared" si="1"/>
-        <v>0.9170366662</v>
+        <v>0.9718605532</v>
       </c>
       <c r="C8" s="68">
         <v>786938.0</v>
       </c>
       <c r="D8" s="69">
-        <v>721651.0</v>
+        <v>764794.0</v>
       </c>
       <c r="E8" s="65"/>
       <c r="F8" s="66">
@@ -1709,13 +1718,13 @@
       </c>
       <c r="B9" s="67">
         <f t="shared" si="1"/>
-        <v>1.136868565</v>
+        <v>1.133095043</v>
       </c>
       <c r="C9" s="69">
         <v>848544.0</v>
       </c>
       <c r="D9" s="69">
-        <v>964683.0</v>
+        <v>961481.0</v>
       </c>
       <c r="E9" s="65"/>
       <c r="F9" s="66">
@@ -1728,13 +1737,13 @@
       </c>
       <c r="B10" s="67">
         <f t="shared" si="1"/>
-        <v>1.858636324</v>
+        <v>1.858407406</v>
       </c>
       <c r="C10" s="69">
         <v>921729.0</v>
       </c>
       <c r="D10" s="69">
-        <v>1713159.0</v>
+        <v>1712948.0</v>
       </c>
       <c r="E10" s="65"/>
       <c r="F10" s="66">
@@ -1747,13 +1756,13 @@
       </c>
       <c r="B11" s="67">
         <f t="shared" si="1"/>
-        <v>2.95823873</v>
+        <v>2.957661543</v>
       </c>
       <c r="C11" s="69">
         <v>966757.0</v>
       </c>
       <c r="D11" s="69">
-        <v>2859898.0</v>
+        <v>2859340.0</v>
       </c>
       <c r="E11" s="65"/>
       <c r="F11" s="66">
@@ -1766,13 +1775,13 @@
       </c>
       <c r="B12" s="67">
         <f t="shared" si="1"/>
-        <v>3.365783825</v>
+        <v>3.379891483</v>
       </c>
       <c r="C12" s="69">
         <v>1018454.0</v>
       </c>
       <c r="D12" s="69">
-        <v>3427896.0</v>
+        <v>3442264.0</v>
       </c>
       <c r="E12" s="70" t="s">
         <v>8</v>
@@ -1787,13 +1796,13 @@
       </c>
       <c r="B13" s="67">
         <f t="shared" si="1"/>
-        <v>2.844603247</v>
+        <v>2.844248328</v>
       </c>
       <c r="C13" s="69">
         <v>1005864.0</v>
       </c>
       <c r="D13" s="69">
-        <v>2861284.0</v>
+        <v>2860927.0</v>
       </c>
       <c r="E13" s="65"/>
       <c r="F13" s="66">
@@ -1806,13 +1815,13 @@
       </c>
       <c r="B14" s="67">
         <f t="shared" si="1"/>
-        <v>1.906295215</v>
+        <v>1.905906347</v>
       </c>
       <c r="C14" s="69">
         <v>966909.0</v>
       </c>
       <c r="D14" s="69">
-        <v>1843214.0</v>
+        <v>1842838.0</v>
       </c>
       <c r="E14" s="65"/>
       <c r="F14" s="66">
@@ -1825,13 +1834,13 @@
       </c>
       <c r="B15" s="67">
         <f t="shared" si="1"/>
-        <v>1.062533992</v>
+        <v>1.063593354</v>
       </c>
       <c r="C15" s="69">
         <v>915646.0</v>
       </c>
       <c r="D15" s="69">
-        <v>972905.0</v>
+        <v>973875.0</v>
       </c>
       <c r="E15" s="65"/>
       <c r="F15" s="66">
@@ -1844,13 +1853,13 @@
       </c>
       <c r="B16" s="67">
         <f t="shared" si="1"/>
-        <v>0.3389862554</v>
+        <v>0.3414012739</v>
       </c>
       <c r="C16" s="69">
         <v>745750.0</v>
       </c>
       <c r="D16" s="69">
-        <v>252799.0</v>
+        <v>254600.0</v>
       </c>
       <c r="E16" s="65"/>
       <c r="F16" s="66">
@@ -1863,13 +1872,13 @@
       </c>
       <c r="B17" s="71">
         <f t="shared" si="1"/>
-        <v>1.268254153</v>
+        <v>1.258902751</v>
       </c>
       <c r="C17" s="72">
         <v>739996.0</v>
       </c>
       <c r="D17" s="72">
-        <v>938503.0</v>
+        <v>931583.0</v>
       </c>
       <c r="E17" s="73"/>
       <c r="F17" s="66">
@@ -1882,17 +1891,17 @@
       </c>
       <c r="B18" s="62">
         <f t="shared" si="1"/>
-        <v>0.5040012611</v>
+        <v>0.5024975326</v>
       </c>
       <c r="C18" s="64">
         <v>729520.0</v>
       </c>
       <c r="D18" s="64">
-        <v>367679.0</v>
+        <v>366582.0</v>
       </c>
       <c r="E18" s="74">
         <f>D18/C18</f>
-        <v>0.5040012611</v>
+        <v>0.5024975326</v>
       </c>
       <c r="F18" s="75">
         <v>1.0</v>
@@ -1904,17 +1913,17 @@
       </c>
       <c r="B19" s="67">
         <f t="shared" si="1"/>
-        <v>0.858693072</v>
+        <v>0.8431746872</v>
       </c>
       <c r="C19" s="69">
         <v>695111.0</v>
       </c>
       <c r="D19" s="69">
-        <v>596887.0</v>
+        <v>586100.0</v>
       </c>
       <c r="E19" s="67">
         <f t="shared" ref="E19:E29" si="2">sum(D$18:D19)/sum(C$18:C19)</f>
-        <v>0.6770637449</v>
+        <v>0.6687219357</v>
       </c>
       <c r="F19" s="76">
         <v>1.0</v>
@@ -1926,17 +1935,17 @@
       </c>
       <c r="B20" s="67">
         <f t="shared" si="1"/>
-        <v>1.323814864</v>
+        <v>1.318724928</v>
       </c>
       <c r="C20" s="69">
         <v>463660.0</v>
       </c>
       <c r="D20" s="69">
-        <v>613800.0</v>
+        <v>611440.0</v>
       </c>
       <c r="E20" s="67">
         <f t="shared" si="2"/>
-        <v>0.8358701069</v>
+        <v>0.828326778</v>
       </c>
       <c r="F20" s="76">
         <v>1.0</v>
@@ -1948,17 +1957,17 @@
       </c>
       <c r="B21" s="67">
         <f t="shared" si="1"/>
-        <v>0.003404032469</v>
+        <v>0.001483809025</v>
       </c>
       <c r="C21" s="69">
         <v>103113.0</v>
       </c>
       <c r="D21" s="69">
-        <v>351.0</v>
+        <v>153.0</v>
       </c>
       <c r="E21" s="67">
         <f t="shared" si="2"/>
-        <v>0.7927658074</v>
+        <v>0.7855136376</v>
       </c>
       <c r="F21" s="76">
         <v>1.0</v>
@@ -1970,17 +1979,17 @@
       </c>
       <c r="B22" s="67">
         <f t="shared" si="1"/>
-        <v>0.0299100371</v>
+        <v>0.02324166829</v>
       </c>
       <c r="C22" s="69">
         <v>133166.0</v>
       </c>
       <c r="D22" s="69">
-        <v>3983.0</v>
+        <v>3095.0</v>
       </c>
       <c r="E22" s="67">
         <f t="shared" si="2"/>
-        <v>0.744950743</v>
+        <v>0.7377351652</v>
       </c>
       <c r="F22" s="76">
         <v>1.0</v>
@@ -1992,17 +2001,17 @@
       </c>
       <c r="B23" s="67">
         <f t="shared" si="1"/>
-        <v>0.01775360153</v>
+        <v>0.01531771176</v>
       </c>
       <c r="C23" s="69">
         <v>200748.0</v>
       </c>
       <c r="D23" s="69">
-        <v>3564.0</v>
+        <v>3075.0</v>
       </c>
       <c r="E23" s="67">
         <f t="shared" si="2"/>
-        <v>0.6821707827</v>
+        <v>0.6753678422</v>
       </c>
       <c r="F23" s="76">
         <v>1.0</v>
@@ -2024,7 +2033,7 @@
       </c>
       <c r="E24" s="67">
         <f t="shared" si="2"/>
-        <v>0.5845797355</v>
+        <v>0.5787761143</v>
       </c>
       <c r="F24" s="76">
         <v>1.0</v>
@@ -2036,17 +2045,17 @@
       </c>
       <c r="B25" s="67">
         <f t="shared" si="1"/>
-        <v>0.01764158179</v>
+        <v>0.01723550958</v>
       </c>
       <c r="C25" s="69">
         <v>487598.0</v>
       </c>
       <c r="D25" s="69">
-        <v>8602.0</v>
+        <v>8404.0</v>
       </c>
       <c r="E25" s="67">
         <f t="shared" si="2"/>
-        <v>0.4985507156</v>
+        <v>0.4935661359</v>
       </c>
       <c r="F25" s="76">
         <v>1.0</v>
@@ -2058,17 +2067,17 @@
       </c>
       <c r="B26" s="67">
         <f t="shared" si="1"/>
-        <v>0.007893165434</v>
+        <v>0.007087833772</v>
       </c>
       <c r="C26" s="69">
         <v>437087.0</v>
       </c>
       <c r="D26" s="69">
-        <v>3450.0</v>
+        <v>3098.0</v>
       </c>
       <c r="E26" s="67">
         <f t="shared" si="2"/>
-        <v>0.4398009312</v>
+        <v>0.4353167614</v>
       </c>
       <c r="F26" s="76">
         <v>1.0</v>
@@ -2080,17 +2089,17 @@
       </c>
       <c r="B27" s="67">
         <f t="shared" si="1"/>
-        <v>0.02614268502</v>
+        <v>0.02438411649</v>
       </c>
       <c r="C27" s="69">
         <v>390090.0</v>
       </c>
       <c r="D27" s="69">
-        <v>10198.0</v>
+        <v>9512.0</v>
       </c>
       <c r="E27" s="67">
         <f t="shared" si="2"/>
-        <v>0.3998641748</v>
+        <v>0.395643149</v>
       </c>
       <c r="F27" s="76">
         <v>1.0</v>
@@ -2102,17 +2111,17 @@
       </c>
       <c r="B28" s="67">
         <f t="shared" si="1"/>
-        <v>0.01232684026</v>
+        <v>0.01278968436</v>
       </c>
       <c r="C28" s="69">
         <v>276551.0</v>
       </c>
       <c r="D28" s="69">
-        <v>3409.0</v>
+        <v>3537.0</v>
       </c>
       <c r="E28" s="67">
         <f t="shared" si="2"/>
-        <v>0.3750383944</v>
+        <v>0.3711174189</v>
       </c>
       <c r="F28" s="76">
         <v>1.0</v>
@@ -2124,17 +2133,17 @@
       </c>
       <c r="B29" s="71">
         <f t="shared" si="1"/>
-        <v>0.007053501045</v>
+        <v>0.00596017411</v>
       </c>
       <c r="C29" s="72">
         <v>291770.0</v>
       </c>
       <c r="D29" s="72">
-        <v>2058.0</v>
+        <v>1739.0</v>
       </c>
       <c r="E29" s="71">
         <f t="shared" si="2"/>
-        <v>0.3517423594</v>
+        <v>0.348000394</v>
       </c>
       <c r="F29" s="77">
         <v>1.0</v>
@@ -2672,7 +2681,7 @@
         <v>4</v>
       </c>
       <c r="B2" s="10">
-        <v>44209.0</v>
+        <v>44308.0</v>
       </c>
       <c r="C2" s="11" t="s">
         <v>5</v>
@@ -2742,15 +2751,15 @@
         <v>4608808.0</v>
       </c>
       <c r="D6" s="95">
-        <v>1621113.0</v>
+        <v>1603867.0</v>
       </c>
       <c r="E6" s="94">
         <f t="shared" ref="E6:E15" si="1">D6/C6</f>
-        <v>0.3517423594</v>
+        <v>0.348000394</v>
       </c>
       <c r="F6" s="94">
         <f>E6-B6</f>
-        <v>-0.5482576406</v>
+        <v>-0.551999606</v>
       </c>
     </row>
     <row r="7" ht="12.75" customHeight="1">
@@ -2847,11 +2856,11 @@
         <v>2718800.0</v>
       </c>
       <c r="D12" s="95">
-        <v>1114831.0</v>
+        <v>1123780.0</v>
       </c>
       <c r="E12" s="94">
         <f t="shared" si="1"/>
-        <v>0.4100452405</v>
+        <v>0.4133367662</v>
       </c>
       <c r="F12" s="94"/>
     </row>
@@ -2864,11 +2873,11 @@
         <v>556413.0</v>
       </c>
       <c r="D13" s="95">
-        <v>3148.0</v>
+        <v>3420.0</v>
       </c>
       <c r="E13" s="94">
         <f t="shared" si="1"/>
-        <v>0.005657667955</v>
+        <v>0.006146513471</v>
       </c>
       <c r="F13" s="94"/>
     </row>
@@ -2881,11 +2890,11 @@
         <v>885135.0</v>
       </c>
       <c r="D14" s="95">
-        <v>432193.0</v>
+        <v>405726.0</v>
       </c>
       <c r="E14" s="94">
         <f t="shared" si="1"/>
-        <v>0.4882791891</v>
+        <v>0.4583775356</v>
       </c>
       <c r="F14" s="94"/>
     </row>
@@ -2954,7 +2963,7 @@
         <v>4</v>
       </c>
       <c r="B2" s="10">
-        <v>44209.0</v>
+        <v>44308.0</v>
       </c>
       <c r="C2" s="11" t="s">
         <v>5</v>
@@ -3178,11 +3187,11 @@
         <v>1389923.0</v>
       </c>
       <c r="D15" s="95">
-        <v>803449.0</v>
+        <v>829916.0</v>
       </c>
       <c r="E15" s="97">
         <f t="shared" si="1"/>
-        <v>0.5780528849</v>
+        <v>0.597094947</v>
       </c>
       <c r="F15" s="94"/>
     </row>
@@ -3348,11 +3357,11 @@
         <v>346312.0</v>
       </c>
       <c r="D25" s="95">
-        <v>3148.0</v>
+        <v>3420.0</v>
       </c>
       <c r="E25" s="97">
         <f t="shared" si="1"/>
-        <v>0.009090069071</v>
+        <v>0.009875487999</v>
       </c>
       <c r="F25" s="94"/>
     </row>
@@ -3450,11 +3459,11 @@
         <v>853599.0</v>
       </c>
       <c r="D31" s="95">
-        <v>364698.0</v>
+        <v>338231.0</v>
       </c>
       <c r="E31" s="97">
         <f t="shared" si="1"/>
-        <v>0.4272474546</v>
+        <v>0.3962410921</v>
       </c>
       <c r="F31" s="94"/>
     </row>
@@ -3484,11 +3493,11 @@
         <v>477046.0</v>
       </c>
       <c r="D33" s="95">
-        <v>36821.0</v>
+        <v>19303.0</v>
       </c>
       <c r="E33" s="97">
         <f t="shared" si="1"/>
-        <v>0.07718542866</v>
+        <v>0.04046360309</v>
       </c>
       <c r="F33" s="94"/>
     </row>
@@ -3545,28 +3554,36 @@
       </c>
     </row>
     <row r="2" ht="15.75" customHeight="1">
-      <c r="A2" s="99"/>
-      <c r="B2" s="100"/>
-      <c r="C2" s="101"/>
-      <c r="D2" s="100"/>
+      <c r="A2" s="99">
+        <v>44308.0</v>
+      </c>
+      <c r="B2" s="100" t="s">
+        <v>158</v>
+      </c>
+      <c r="C2" s="101">
+        <v>2020.0</v>
+      </c>
+      <c r="D2" s="100" t="s">
+        <v>159</v>
+      </c>
     </row>
     <row r="3" ht="15.75" customHeight="1">
-      <c r="A3" s="99"/>
+      <c r="A3" s="102"/>
       <c r="B3" s="100"/>
-      <c r="C3" s="101"/>
+      <c r="C3" s="103"/>
       <c r="D3" s="100"/>
     </row>
     <row r="4" ht="15.75" customHeight="1">
-      <c r="A4" s="99"/>
+      <c r="A4" s="102"/>
       <c r="B4" s="100"/>
-      <c r="C4" s="102"/>
+      <c r="C4" s="104"/>
       <c r="D4" s="100"/>
     </row>
     <row r="5" ht="15.75" customHeight="1">
-      <c r="A5" s="103"/>
-      <c r="B5" s="104"/>
-      <c r="C5" s="101"/>
-      <c r="D5" s="105"/>
+      <c r="A5" s="99"/>
+      <c r="B5" s="105"/>
+      <c r="C5" s="103"/>
+      <c r="D5" s="106"/>
     </row>
   </sheetData>
   <drawing r:id="rId1"/>

</xml_diff>

<commit_message>
post ops update 2020 (#39)
</commit_message>
<xml_diff>
--- a/static/download/2020/RP3_ERT_ATFM_2020_Jan_Dec.xlsx
+++ b/static/download/2020/RP3_ERT_ATFM_2020_Jan_Dec.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="212" uniqueCount="158">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="214" uniqueCount="160">
   <si>
     <t>Data source</t>
   </si>
@@ -489,6 +489,12 @@
   </si>
   <si>
     <t>Comment</t>
+  </si>
+  <si>
+    <t>All</t>
+  </si>
+  <si>
+    <t>Data updated with post-ops adjustments</t>
   </si>
 </sst>
 </file>
@@ -843,7 +849,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="106">
+  <cellXfs count="107">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -1138,19 +1144,22 @@
       <alignment shrinkToFit="0" wrapText="0"/>
     </xf>
     <xf borderId="0" fillId="3" fontId="10" numFmtId="164" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
-      <alignment horizontal="center" shrinkToFit="0" vertical="bottom" wrapText="0"/>
+      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
     <xf borderId="0" fillId="3" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
     <xf borderId="0" fillId="3" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
+    </xf>
+    <xf borderId="0" fillId="3" fontId="10" numFmtId="164" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
+      <alignment horizontal="center" shrinkToFit="0" vertical="bottom" wrapText="0"/>
+    </xf>
+    <xf borderId="0" fillId="3" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="center" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="10" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0" shrinkToFit="0" wrapText="0"/>
-    </xf>
-    <xf borderId="0" fillId="3" fontId="10" numFmtId="164" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
-      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
     <xf borderId="0" fillId="3" fontId="6" numFmtId="17" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
       <alignment vertical="bottom"/>
@@ -1234,7 +1243,7 @@
         <v>4</v>
       </c>
       <c r="B2" s="10">
-        <v>44209.0</v>
+        <v>44308.0</v>
       </c>
       <c r="C2" s="11" t="s">
         <v>5</v>
@@ -1450,20 +1459,20 @@
       </c>
       <c r="C11" s="31">
         <f t="shared" si="1"/>
-        <v>0.3517423594</v>
+        <v>0.348000394</v>
       </c>
       <c r="D11" s="38">
         <v>4608808.0</v>
       </c>
       <c r="E11" s="39">
-        <v>1621113.0</v>
+        <v>1603867.0</v>
       </c>
       <c r="F11" s="42">
         <v>0.9</v>
       </c>
       <c r="G11" s="41">
         <f t="shared" si="2"/>
-        <v>-0.5482576406</v>
+        <v>-0.551999606</v>
       </c>
       <c r="H11" s="36">
         <v>0.0071</v>
@@ -1587,7 +1596,7 @@
         <v>4</v>
       </c>
       <c r="B2" s="10">
-        <v>44209.0</v>
+        <v>44308.0</v>
       </c>
       <c r="C2" s="11" t="s">
         <v>5</v>
@@ -1652,13 +1661,13 @@
       </c>
       <c r="B6" s="62">
         <f t="shared" ref="B6:B29" si="1">D6/C6</f>
-        <v>0.3901494621</v>
+        <v>0.3881771646</v>
       </c>
       <c r="C6" s="63">
         <v>730620.0</v>
       </c>
       <c r="D6" s="64">
-        <v>285051.0</v>
+        <v>283610.0</v>
       </c>
       <c r="E6" s="65"/>
       <c r="F6" s="66">
@@ -1671,13 +1680,13 @@
       </c>
       <c r="B7" s="67">
         <f t="shared" si="1"/>
-        <v>0.489219714</v>
+        <v>0.4865745041</v>
       </c>
       <c r="C7" s="68">
         <v>686902.0</v>
       </c>
       <c r="D7" s="69">
-        <v>336046.0</v>
+        <v>334229.0</v>
       </c>
       <c r="E7" s="65"/>
       <c r="F7" s="66">
@@ -1690,13 +1699,13 @@
       </c>
       <c r="B8" s="67">
         <f t="shared" si="1"/>
-        <v>0.9170366662</v>
+        <v>0.9718605532</v>
       </c>
       <c r="C8" s="68">
         <v>786938.0</v>
       </c>
       <c r="D8" s="69">
-        <v>721651.0</v>
+        <v>764794.0</v>
       </c>
       <c r="E8" s="65"/>
       <c r="F8" s="66">
@@ -1709,13 +1718,13 @@
       </c>
       <c r="B9" s="67">
         <f t="shared" si="1"/>
-        <v>1.136868565</v>
+        <v>1.133095043</v>
       </c>
       <c r="C9" s="69">
         <v>848544.0</v>
       </c>
       <c r="D9" s="69">
-        <v>964683.0</v>
+        <v>961481.0</v>
       </c>
       <c r="E9" s="65"/>
       <c r="F9" s="66">
@@ -1728,13 +1737,13 @@
       </c>
       <c r="B10" s="67">
         <f t="shared" si="1"/>
-        <v>1.858636324</v>
+        <v>1.858407406</v>
       </c>
       <c r="C10" s="69">
         <v>921729.0</v>
       </c>
       <c r="D10" s="69">
-        <v>1713159.0</v>
+        <v>1712948.0</v>
       </c>
       <c r="E10" s="65"/>
       <c r="F10" s="66">
@@ -1747,13 +1756,13 @@
       </c>
       <c r="B11" s="67">
         <f t="shared" si="1"/>
-        <v>2.95823873</v>
+        <v>2.957661543</v>
       </c>
       <c r="C11" s="69">
         <v>966757.0</v>
       </c>
       <c r="D11" s="69">
-        <v>2859898.0</v>
+        <v>2859340.0</v>
       </c>
       <c r="E11" s="65"/>
       <c r="F11" s="66">
@@ -1766,13 +1775,13 @@
       </c>
       <c r="B12" s="67">
         <f t="shared" si="1"/>
-        <v>3.365783825</v>
+        <v>3.379891483</v>
       </c>
       <c r="C12" s="69">
         <v>1018454.0</v>
       </c>
       <c r="D12" s="69">
-        <v>3427896.0</v>
+        <v>3442264.0</v>
       </c>
       <c r="E12" s="70" t="s">
         <v>8</v>
@@ -1787,13 +1796,13 @@
       </c>
       <c r="B13" s="67">
         <f t="shared" si="1"/>
-        <v>2.844603247</v>
+        <v>2.844248328</v>
       </c>
       <c r="C13" s="69">
         <v>1005864.0</v>
       </c>
       <c r="D13" s="69">
-        <v>2861284.0</v>
+        <v>2860927.0</v>
       </c>
       <c r="E13" s="65"/>
       <c r="F13" s="66">
@@ -1806,13 +1815,13 @@
       </c>
       <c r="B14" s="67">
         <f t="shared" si="1"/>
-        <v>1.906295215</v>
+        <v>1.905906347</v>
       </c>
       <c r="C14" s="69">
         <v>966909.0</v>
       </c>
       <c r="D14" s="69">
-        <v>1843214.0</v>
+        <v>1842838.0</v>
       </c>
       <c r="E14" s="65"/>
       <c r="F14" s="66">
@@ -1825,13 +1834,13 @@
       </c>
       <c r="B15" s="67">
         <f t="shared" si="1"/>
-        <v>1.062533992</v>
+        <v>1.063593354</v>
       </c>
       <c r="C15" s="69">
         <v>915646.0</v>
       </c>
       <c r="D15" s="69">
-        <v>972905.0</v>
+        <v>973875.0</v>
       </c>
       <c r="E15" s="65"/>
       <c r="F15" s="66">
@@ -1844,13 +1853,13 @@
       </c>
       <c r="B16" s="67">
         <f t="shared" si="1"/>
-        <v>0.3389862554</v>
+        <v>0.3414012739</v>
       </c>
       <c r="C16" s="69">
         <v>745750.0</v>
       </c>
       <c r="D16" s="69">
-        <v>252799.0</v>
+        <v>254600.0</v>
       </c>
       <c r="E16" s="65"/>
       <c r="F16" s="66">
@@ -1863,13 +1872,13 @@
       </c>
       <c r="B17" s="71">
         <f t="shared" si="1"/>
-        <v>1.268254153</v>
+        <v>1.258902751</v>
       </c>
       <c r="C17" s="72">
         <v>739996.0</v>
       </c>
       <c r="D17" s="72">
-        <v>938503.0</v>
+        <v>931583.0</v>
       </c>
       <c r="E17" s="73"/>
       <c r="F17" s="66">
@@ -1882,17 +1891,17 @@
       </c>
       <c r="B18" s="62">
         <f t="shared" si="1"/>
-        <v>0.5040012611</v>
+        <v>0.5024975326</v>
       </c>
       <c r="C18" s="64">
         <v>729520.0</v>
       </c>
       <c r="D18" s="64">
-        <v>367679.0</v>
+        <v>366582.0</v>
       </c>
       <c r="E18" s="74">
         <f>D18/C18</f>
-        <v>0.5040012611</v>
+        <v>0.5024975326</v>
       </c>
       <c r="F18" s="75">
         <v>1.0</v>
@@ -1904,17 +1913,17 @@
       </c>
       <c r="B19" s="67">
         <f t="shared" si="1"/>
-        <v>0.858693072</v>
+        <v>0.8431746872</v>
       </c>
       <c r="C19" s="69">
         <v>695111.0</v>
       </c>
       <c r="D19" s="69">
-        <v>596887.0</v>
+        <v>586100.0</v>
       </c>
       <c r="E19" s="67">
         <f t="shared" ref="E19:E29" si="2">sum(D$18:D19)/sum(C$18:C19)</f>
-        <v>0.6770637449</v>
+        <v>0.6687219357</v>
       </c>
       <c r="F19" s="76">
         <v>1.0</v>
@@ -1926,17 +1935,17 @@
       </c>
       <c r="B20" s="67">
         <f t="shared" si="1"/>
-        <v>1.323814864</v>
+        <v>1.318724928</v>
       </c>
       <c r="C20" s="69">
         <v>463660.0</v>
       </c>
       <c r="D20" s="69">
-        <v>613800.0</v>
+        <v>611440.0</v>
       </c>
       <c r="E20" s="67">
         <f t="shared" si="2"/>
-        <v>0.8358701069</v>
+        <v>0.828326778</v>
       </c>
       <c r="F20" s="76">
         <v>1.0</v>
@@ -1948,17 +1957,17 @@
       </c>
       <c r="B21" s="67">
         <f t="shared" si="1"/>
-        <v>0.003404032469</v>
+        <v>0.001483809025</v>
       </c>
       <c r="C21" s="69">
         <v>103113.0</v>
       </c>
       <c r="D21" s="69">
-        <v>351.0</v>
+        <v>153.0</v>
       </c>
       <c r="E21" s="67">
         <f t="shared" si="2"/>
-        <v>0.7927658074</v>
+        <v>0.7855136376</v>
       </c>
       <c r="F21" s="76">
         <v>1.0</v>
@@ -1970,17 +1979,17 @@
       </c>
       <c r="B22" s="67">
         <f t="shared" si="1"/>
-        <v>0.0299100371</v>
+        <v>0.02324166829</v>
       </c>
       <c r="C22" s="69">
         <v>133166.0</v>
       </c>
       <c r="D22" s="69">
-        <v>3983.0</v>
+        <v>3095.0</v>
       </c>
       <c r="E22" s="67">
         <f t="shared" si="2"/>
-        <v>0.744950743</v>
+        <v>0.7377351652</v>
       </c>
       <c r="F22" s="76">
         <v>1.0</v>
@@ -1992,17 +2001,17 @@
       </c>
       <c r="B23" s="67">
         <f t="shared" si="1"/>
-        <v>0.01775360153</v>
+        <v>0.01531771176</v>
       </c>
       <c r="C23" s="69">
         <v>200748.0</v>
       </c>
       <c r="D23" s="69">
-        <v>3564.0</v>
+        <v>3075.0</v>
       </c>
       <c r="E23" s="67">
         <f t="shared" si="2"/>
-        <v>0.6821707827</v>
+        <v>0.6753678422</v>
       </c>
       <c r="F23" s="76">
         <v>1.0</v>
@@ -2024,7 +2033,7 @@
       </c>
       <c r="E24" s="67">
         <f t="shared" si="2"/>
-        <v>0.5845797355</v>
+        <v>0.5787761143</v>
       </c>
       <c r="F24" s="76">
         <v>1.0</v>
@@ -2036,17 +2045,17 @@
       </c>
       <c r="B25" s="67">
         <f t="shared" si="1"/>
-        <v>0.01764158179</v>
+        <v>0.01723550958</v>
       </c>
       <c r="C25" s="69">
         <v>487598.0</v>
       </c>
       <c r="D25" s="69">
-        <v>8602.0</v>
+        <v>8404.0</v>
       </c>
       <c r="E25" s="67">
         <f t="shared" si="2"/>
-        <v>0.4985507156</v>
+        <v>0.4935661359</v>
       </c>
       <c r="F25" s="76">
         <v>1.0</v>
@@ -2058,17 +2067,17 @@
       </c>
       <c r="B26" s="67">
         <f t="shared" si="1"/>
-        <v>0.007893165434</v>
+        <v>0.007087833772</v>
       </c>
       <c r="C26" s="69">
         <v>437087.0</v>
       </c>
       <c r="D26" s="69">
-        <v>3450.0</v>
+        <v>3098.0</v>
       </c>
       <c r="E26" s="67">
         <f t="shared" si="2"/>
-        <v>0.4398009312</v>
+        <v>0.4353167614</v>
       </c>
       <c r="F26" s="76">
         <v>1.0</v>
@@ -2080,17 +2089,17 @@
       </c>
       <c r="B27" s="67">
         <f t="shared" si="1"/>
-        <v>0.02614268502</v>
+        <v>0.02438411649</v>
       </c>
       <c r="C27" s="69">
         <v>390090.0</v>
       </c>
       <c r="D27" s="69">
-        <v>10198.0</v>
+        <v>9512.0</v>
       </c>
       <c r="E27" s="67">
         <f t="shared" si="2"/>
-        <v>0.3998641748</v>
+        <v>0.395643149</v>
       </c>
       <c r="F27" s="76">
         <v>1.0</v>
@@ -2102,17 +2111,17 @@
       </c>
       <c r="B28" s="67">
         <f t="shared" si="1"/>
-        <v>0.01232684026</v>
+        <v>0.01278968436</v>
       </c>
       <c r="C28" s="69">
         <v>276551.0</v>
       </c>
       <c r="D28" s="69">
-        <v>3409.0</v>
+        <v>3537.0</v>
       </c>
       <c r="E28" s="67">
         <f t="shared" si="2"/>
-        <v>0.3750383944</v>
+        <v>0.3711174189</v>
       </c>
       <c r="F28" s="76">
         <v>1.0</v>
@@ -2124,17 +2133,17 @@
       </c>
       <c r="B29" s="71">
         <f t="shared" si="1"/>
-        <v>0.007053501045</v>
+        <v>0.00596017411</v>
       </c>
       <c r="C29" s="72">
         <v>291770.0</v>
       </c>
       <c r="D29" s="72">
-        <v>2058.0</v>
+        <v>1739.0</v>
       </c>
       <c r="E29" s="71">
         <f t="shared" si="2"/>
-        <v>0.3517423594</v>
+        <v>0.348000394</v>
       </c>
       <c r="F29" s="77">
         <v>1.0</v>
@@ -2672,7 +2681,7 @@
         <v>4</v>
       </c>
       <c r="B2" s="10">
-        <v>44209.0</v>
+        <v>44308.0</v>
       </c>
       <c r="C2" s="11" t="s">
         <v>5</v>
@@ -2742,15 +2751,15 @@
         <v>4608808.0</v>
       </c>
       <c r="D6" s="95">
-        <v>1621113.0</v>
+        <v>1603867.0</v>
       </c>
       <c r="E6" s="94">
         <f t="shared" ref="E6:E15" si="1">D6/C6</f>
-        <v>0.3517423594</v>
+        <v>0.348000394</v>
       </c>
       <c r="F6" s="94">
         <f>E6-B6</f>
-        <v>-0.5482576406</v>
+        <v>-0.551999606</v>
       </c>
     </row>
     <row r="7" ht="12.75" customHeight="1">
@@ -2847,11 +2856,11 @@
         <v>2718800.0</v>
       </c>
       <c r="D12" s="95">
-        <v>1114831.0</v>
+        <v>1123780.0</v>
       </c>
       <c r="E12" s="94">
         <f t="shared" si="1"/>
-        <v>0.4100452405</v>
+        <v>0.4133367662</v>
       </c>
       <c r="F12" s="94"/>
     </row>
@@ -2864,11 +2873,11 @@
         <v>556413.0</v>
       </c>
       <c r="D13" s="95">
-        <v>3148.0</v>
+        <v>3420.0</v>
       </c>
       <c r="E13" s="94">
         <f t="shared" si="1"/>
-        <v>0.005657667955</v>
+        <v>0.006146513471</v>
       </c>
       <c r="F13" s="94"/>
     </row>
@@ -2881,11 +2890,11 @@
         <v>885135.0</v>
       </c>
       <c r="D14" s="95">
-        <v>432193.0</v>
+        <v>405726.0</v>
       </c>
       <c r="E14" s="94">
         <f t="shared" si="1"/>
-        <v>0.4882791891</v>
+        <v>0.4583775356</v>
       </c>
       <c r="F14" s="94"/>
     </row>
@@ -2954,7 +2963,7 @@
         <v>4</v>
       </c>
       <c r="B2" s="10">
-        <v>44209.0</v>
+        <v>44308.0</v>
       </c>
       <c r="C2" s="11" t="s">
         <v>5</v>
@@ -3178,11 +3187,11 @@
         <v>1389923.0</v>
       </c>
       <c r="D15" s="95">
-        <v>803449.0</v>
+        <v>829916.0</v>
       </c>
       <c r="E15" s="97">
         <f t="shared" si="1"/>
-        <v>0.5780528849</v>
+        <v>0.597094947</v>
       </c>
       <c r="F15" s="94"/>
     </row>
@@ -3348,11 +3357,11 @@
         <v>346312.0</v>
       </c>
       <c r="D25" s="95">
-        <v>3148.0</v>
+        <v>3420.0</v>
       </c>
       <c r="E25" s="97">
         <f t="shared" si="1"/>
-        <v>0.009090069071</v>
+        <v>0.009875487999</v>
       </c>
       <c r="F25" s="94"/>
     </row>
@@ -3450,11 +3459,11 @@
         <v>853599.0</v>
       </c>
       <c r="D31" s="95">
-        <v>364698.0</v>
+        <v>338231.0</v>
       </c>
       <c r="E31" s="97">
         <f t="shared" si="1"/>
-        <v>0.4272474546</v>
+        <v>0.3962410921</v>
       </c>
       <c r="F31" s="94"/>
     </row>
@@ -3484,11 +3493,11 @@
         <v>477046.0</v>
       </c>
       <c r="D33" s="95">
-        <v>36821.0</v>
+        <v>19303.0</v>
       </c>
       <c r="E33" s="97">
         <f t="shared" si="1"/>
-        <v>0.07718542866</v>
+        <v>0.04046360309</v>
       </c>
       <c r="F33" s="94"/>
     </row>
@@ -3545,28 +3554,36 @@
       </c>
     </row>
     <row r="2" ht="15.75" customHeight="1">
-      <c r="A2" s="99"/>
-      <c r="B2" s="100"/>
-      <c r="C2" s="101"/>
-      <c r="D2" s="100"/>
+      <c r="A2" s="99">
+        <v>44308.0</v>
+      </c>
+      <c r="B2" s="100" t="s">
+        <v>158</v>
+      </c>
+      <c r="C2" s="101">
+        <v>2020.0</v>
+      </c>
+      <c r="D2" s="100" t="s">
+        <v>159</v>
+      </c>
     </row>
     <row r="3" ht="15.75" customHeight="1">
-      <c r="A3" s="99"/>
+      <c r="A3" s="102"/>
       <c r="B3" s="100"/>
-      <c r="C3" s="101"/>
+      <c r="C3" s="103"/>
       <c r="D3" s="100"/>
     </row>
     <row r="4" ht="15.75" customHeight="1">
-      <c r="A4" s="99"/>
+      <c r="A4" s="102"/>
       <c r="B4" s="100"/>
-      <c r="C4" s="102"/>
+      <c r="C4" s="104"/>
       <c r="D4" s="100"/>
     </row>
     <row r="5" ht="15.75" customHeight="1">
-      <c r="A5" s="103"/>
-      <c r="B5" s="104"/>
-      <c r="C5" s="101"/>
-      <c r="D5" s="105"/>
+      <c r="A5" s="99"/>
+      <c r="B5" s="105"/>
+      <c r="C5" s="103"/>
+      <c r="D5" s="106"/>
     </row>
   </sheetData>
   <drawing r:id="rId1"/>

</xml_diff>

<commit_message>
data updates ex SU
</commit_message>
<xml_diff>
--- a/static/download/2020/RP3_ERT_ATFM_2020_Jan_Dec.xlsx
+++ b/static/download/2020/RP3_ERT_ATFM_2020_Jan_Dec.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="214" uniqueCount="160">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="215" uniqueCount="159">
   <si>
     <t>Data source</t>
   </si>
@@ -335,10 +335,10 @@
     <t>Full Year</t>
   </si>
   <si>
-    <t>FAB_FIR</t>
-  </si>
-  <si>
-    <t>FAB (based on FIR)</t>
+    <t>FAB_ANSP</t>
+  </si>
+  <si>
+    <t>FAB (based on ANSP)</t>
   </si>
   <si>
     <t>Plan [2020]</t>
@@ -386,105 +386,99 @@
     <t>UK-Ireland FAB</t>
   </si>
   <si>
-    <t>FIR</t>
-  </si>
-  <si>
-    <t>National (based on FIR)</t>
-  </si>
-  <si>
-    <t>Austria</t>
-  </si>
-  <si>
-    <t>Belgium</t>
-  </si>
-  <si>
-    <t>Bulgaria</t>
-  </si>
-  <si>
-    <t>Croatia</t>
-  </si>
-  <si>
-    <t>Cyprus</t>
-  </si>
-  <si>
-    <t>Czech Republic</t>
-  </si>
-  <si>
-    <t>Denmark</t>
-  </si>
-  <si>
-    <t>Estonia</t>
-  </si>
-  <si>
-    <t>Finland</t>
-  </si>
-  <si>
-    <t>France</t>
-  </si>
-  <si>
-    <t>Germany</t>
-  </si>
-  <si>
-    <t>Greece</t>
-  </si>
-  <si>
-    <t>Hungary</t>
-  </si>
-  <si>
-    <t>Ireland</t>
-  </si>
-  <si>
-    <t>Italy</t>
-  </si>
-  <si>
-    <t>Latvia</t>
-  </si>
-  <si>
-    <t>Lithuania</t>
-  </si>
-  <si>
-    <t>Malta</t>
-  </si>
-  <si>
-    <t>Netherlands</t>
-  </si>
-  <si>
-    <t>Norway</t>
-  </si>
-  <si>
-    <t>Poland</t>
-  </si>
-  <si>
-    <t>Portugal</t>
-  </si>
-  <si>
-    <t>Romania</t>
-  </si>
-  <si>
-    <t>Slovakia</t>
-  </si>
-  <si>
-    <t>Slovenia</t>
-  </si>
-  <si>
-    <t>Spain</t>
-  </si>
-  <si>
-    <t>Sweden</t>
-  </si>
-  <si>
-    <t>Switzerland</t>
-  </si>
-  <si>
-    <t>United Kingdom</t>
+    <t>Entity</t>
+  </si>
+  <si>
+    <t>Austro Control</t>
+  </si>
+  <si>
+    <t>skeyes</t>
+  </si>
+  <si>
+    <t>BULATSA</t>
+  </si>
+  <si>
+    <t>Croatia Control</t>
+  </si>
+  <si>
+    <t>DCAC Cyprus</t>
+  </si>
+  <si>
+    <t>ANS CR</t>
+  </si>
+  <si>
+    <t>NAVIAIR</t>
+  </si>
+  <si>
+    <t>EANS</t>
+  </si>
+  <si>
+    <t>Fintraffic ANS</t>
+  </si>
+  <si>
+    <t>DSNA</t>
+  </si>
+  <si>
+    <t>DFS</t>
+  </si>
+  <si>
+    <t>HCAA</t>
+  </si>
+  <si>
+    <t>HungaroControl (EC)</t>
+  </si>
+  <si>
+    <t>IAA</t>
+  </si>
+  <si>
+    <t>ENAV</t>
+  </si>
+  <si>
+    <t>LGS</t>
+  </si>
+  <si>
+    <t>Oro navigacija</t>
+  </si>
+  <si>
+    <t>MATS</t>
+  </si>
+  <si>
+    <t>LVNL</t>
+  </si>
+  <si>
+    <t>Avinor</t>
+  </si>
+  <si>
+    <t>PANSA</t>
+  </si>
+  <si>
+    <t>NAV Portugal</t>
+  </si>
+  <si>
+    <t>ROMATSA</t>
+  </si>
+  <si>
+    <t>LPS</t>
+  </si>
+  <si>
+    <t>Slovenia Control</t>
+  </si>
+  <si>
+    <t>ENAIRE</t>
+  </si>
+  <si>
+    <t>LFV</t>
+  </si>
+  <si>
+    <t>Skyguide</t>
+  </si>
+  <si>
+    <t>NATS (Continental)</t>
   </si>
   <si>
     <t>Change date</t>
   </si>
   <si>
-    <t>Entity</t>
-  </si>
-  <si>
     <t>Period</t>
   </si>
   <si>
@@ -495,17 +489,21 @@
   </si>
   <si>
     <t>Data updated with post-ops adjustments</t>
+  </si>
+  <si>
+    <t>Local level changed to ANSP</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <numFmts count="4">
+  <numFmts count="5">
     <numFmt numFmtId="164" formatCode="d&quot; &quot;mmm&quot; &quot;yyyy"/>
     <numFmt numFmtId="165" formatCode="m/d/yyyy"/>
     <numFmt numFmtId="166" formatCode="d mmm yyyy"/>
     <numFmt numFmtId="167" formatCode="d mmm. yyyy"/>
+    <numFmt numFmtId="168" formatCode="d mmmm yyyy"/>
   </numFmts>
   <fonts count="21">
     <font>
@@ -849,7 +847,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="107">
+  <cellXfs count="108">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -1104,6 +1102,9 @@
     <xf borderId="5" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment shrinkToFit="0" wrapText="0"/>
     </xf>
+    <xf borderId="5" fillId="3" fontId="4" numFmtId="168" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+      <alignment horizontal="left" readingOrder="0" vertical="bottom"/>
+    </xf>
     <xf borderId="5" fillId="2" fontId="19" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="left" shrinkToFit="0" wrapText="0"/>
     </xf>
@@ -1155,14 +1156,14 @@
     <xf borderId="0" fillId="3" fontId="10" numFmtId="164" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="center" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
+    <xf borderId="0" fillId="0" fontId="10" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" wrapText="0"/>
+    </xf>
+    <xf borderId="0" fillId="3" fontId="6" numFmtId="17" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
+      <alignment vertical="bottom"/>
+    </xf>
     <xf borderId="0" fillId="3" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="center" shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="10" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" wrapText="0"/>
-    </xf>
-    <xf borderId="0" fillId="3" fontId="6" numFmtId="17" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
-      <alignment vertical="bottom"/>
     </xf>
     <xf borderId="0" fillId="3" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment vertical="bottom"/>
@@ -2680,8 +2681,8 @@
       <c r="A2" s="85" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="10">
-        <v>44308.0</v>
+      <c r="B2" s="86">
+        <v>44328.0</v>
       </c>
       <c r="C2" s="11" t="s">
         <v>5</v>
@@ -2689,7 +2690,7 @@
       <c r="D2" s="12">
         <v>44196.0</v>
       </c>
-      <c r="E2" s="86" t="s">
+      <c r="E2" s="87" t="s">
         <v>6</v>
       </c>
       <c r="F2" s="14" t="s">
@@ -2697,223 +2698,223 @@
       </c>
     </row>
     <row r="3" ht="12.75" customHeight="1">
-      <c r="A3" s="87"/>
-      <c r="B3" s="87"/>
-      <c r="C3" s="87"/>
-      <c r="D3" s="87"/>
-      <c r="E3" s="87"/>
-      <c r="F3" s="88" t="s">
+      <c r="A3" s="88"/>
+      <c r="B3" s="88"/>
+      <c r="C3" s="88"/>
+      <c r="D3" s="88"/>
+      <c r="E3" s="88"/>
+      <c r="F3" s="89" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="4" ht="13.5" customHeight="1">
-      <c r="A4" s="89" t="s">
+      <c r="A4" s="90" t="s">
         <v>9</v>
       </c>
-      <c r="B4" s="90" t="s">
+      <c r="B4" s="91" t="s">
         <v>105</v>
       </c>
-      <c r="C4" s="90" t="s">
+      <c r="C4" s="91" t="s">
         <v>106</v>
       </c>
-      <c r="D4" s="91"/>
-      <c r="E4" s="91"/>
-      <c r="F4" s="91"/>
+      <c r="D4" s="92"/>
+      <c r="E4" s="92"/>
+      <c r="F4" s="92"/>
     </row>
     <row r="5" ht="25.5" customHeight="1">
-      <c r="A5" s="92" t="s">
+      <c r="A5" s="93" t="s">
         <v>107</v>
       </c>
-      <c r="B5" s="92" t="s">
+      <c r="B5" s="93" t="s">
         <v>108</v>
       </c>
-      <c r="C5" s="92" t="s">
+      <c r="C5" s="93" t="s">
         <v>109</v>
       </c>
-      <c r="D5" s="92" t="s">
+      <c r="D5" s="93" t="s">
         <v>110</v>
       </c>
-      <c r="E5" s="92" t="s">
+      <c r="E5" s="93" t="s">
         <v>111</v>
       </c>
-      <c r="F5" s="92" t="s">
+      <c r="F5" s="93" t="s">
         <v>112</v>
       </c>
     </row>
     <row r="6" ht="12.75" customHeight="1">
-      <c r="A6" s="93" t="s">
+      <c r="A6" s="94" t="s">
         <v>113</v>
       </c>
-      <c r="B6" s="94">
+      <c r="B6" s="95">
         <v>0.9</v>
       </c>
-      <c r="C6" s="95">
+      <c r="C6" s="96">
         <v>4608808.0</v>
       </c>
-      <c r="D6" s="95">
+      <c r="D6" s="96">
         <v>1603867.0</v>
       </c>
-      <c r="E6" s="94">
+      <c r="E6" s="95">
         <f t="shared" ref="E6:E15" si="1">D6/C6</f>
         <v>0.348000394</v>
       </c>
-      <c r="F6" s="94">
+      <c r="F6" s="95">
         <f>E6-B6</f>
         <v>-0.551999606</v>
       </c>
     </row>
     <row r="7" ht="12.75" customHeight="1">
-      <c r="A7" s="93" t="s">
+      <c r="A7" s="94" t="s">
         <v>114</v>
       </c>
-      <c r="B7" s="94"/>
-      <c r="C7" s="95">
-        <v>432996.0</v>
-      </c>
-      <c r="D7" s="95">
+      <c r="B7" s="95"/>
+      <c r="C7" s="96">
+        <v>414092.0</v>
+      </c>
+      <c r="D7" s="96">
         <v>1404.0</v>
       </c>
-      <c r="E7" s="94">
-        <f t="shared" si="1"/>
-        <v>0.00324252418</v>
-      </c>
-      <c r="F7" s="94"/>
+      <c r="E7" s="95">
+        <f t="shared" si="1"/>
+        <v>0.003390550892</v>
+      </c>
+      <c r="F7" s="95"/>
     </row>
     <row r="8" ht="12.75" customHeight="1">
-      <c r="A8" s="93" t="s">
+      <c r="A8" s="94" t="s">
         <v>115</v>
       </c>
-      <c r="B8" s="94"/>
-      <c r="C8" s="95">
-        <v>1124698.0</v>
-      </c>
-      <c r="D8" s="95">
+      <c r="B8" s="95"/>
+      <c r="C8" s="96">
+        <v>1084733.0</v>
+      </c>
+      <c r="D8" s="96">
         <v>44335.0</v>
       </c>
-      <c r="E8" s="94">
-        <f t="shared" si="1"/>
-        <v>0.03941947083</v>
-      </c>
-      <c r="F8" s="94"/>
+      <c r="E8" s="95">
+        <f t="shared" si="1"/>
+        <v>0.04087180901</v>
+      </c>
+      <c r="F8" s="95"/>
     </row>
     <row r="9" ht="12.75" customHeight="1">
-      <c r="A9" s="93" t="s">
+      <c r="A9" s="94" t="s">
         <v>116</v>
       </c>
-      <c r="B9" s="94"/>
-      <c r="C9" s="95">
-        <v>458990.0</v>
-      </c>
-      <c r="D9" s="95">
+      <c r="B9" s="95"/>
+      <c r="C9" s="96">
+        <v>458992.0</v>
+      </c>
+      <c r="D9" s="96">
         <v>0.0</v>
       </c>
-      <c r="E9" s="94">
+      <c r="E9" s="95">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="F9" s="94"/>
+      <c r="F9" s="95"/>
     </row>
     <row r="10" ht="12.75" customHeight="1">
-      <c r="A10" s="93" t="s">
+      <c r="A10" s="94" t="s">
         <v>117</v>
       </c>
-      <c r="B10" s="94"/>
-      <c r="C10" s="95">
-        <v>448514.0</v>
-      </c>
-      <c r="D10" s="95">
+      <c r="B10" s="95"/>
+      <c r="C10" s="96">
+        <v>450600.0</v>
+      </c>
+      <c r="D10" s="96">
         <v>2680.0</v>
       </c>
-      <c r="E10" s="94">
-        <f t="shared" si="1"/>
-        <v>0.005975287282</v>
-      </c>
-      <c r="F10" s="94"/>
+      <c r="E10" s="95">
+        <f t="shared" si="1"/>
+        <v>0.005947625388</v>
+      </c>
+      <c r="F10" s="95"/>
     </row>
     <row r="11" ht="12.75" customHeight="1">
-      <c r="A11" s="93" t="s">
+      <c r="A11" s="94" t="s">
         <v>118</v>
       </c>
-      <c r="B11" s="94"/>
-      <c r="C11" s="95">
-        <v>979567.0</v>
-      </c>
-      <c r="D11" s="95">
+      <c r="B11" s="95"/>
+      <c r="C11" s="96">
+        <v>916281.0</v>
+      </c>
+      <c r="D11" s="96">
         <v>1539.0</v>
       </c>
-      <c r="E11" s="94">
-        <f t="shared" si="1"/>
-        <v>0.001571102334</v>
-      </c>
-      <c r="F11" s="94"/>
+      <c r="E11" s="95">
+        <f t="shared" si="1"/>
+        <v>0.001679615751</v>
+      </c>
+      <c r="F11" s="95"/>
     </row>
     <row r="12" ht="12.75" customHeight="1">
-      <c r="A12" s="93" t="s">
+      <c r="A12" s="94" t="s">
         <v>119</v>
       </c>
-      <c r="B12" s="94"/>
-      <c r="C12" s="95">
-        <v>2718800.0</v>
-      </c>
-      <c r="D12" s="95">
+      <c r="B12" s="95"/>
+      <c r="C12" s="96">
+        <v>2696221.0</v>
+      </c>
+      <c r="D12" s="96">
         <v>1123780.0</v>
       </c>
-      <c r="E12" s="94">
-        <f t="shared" si="1"/>
-        <v>0.4133367662</v>
-      </c>
-      <c r="F12" s="94"/>
+      <c r="E12" s="95">
+        <f t="shared" si="1"/>
+        <v>0.4167981779</v>
+      </c>
+      <c r="F12" s="95"/>
     </row>
     <row r="13" ht="12.75" customHeight="1">
-      <c r="A13" s="93" t="s">
+      <c r="A13" s="94" t="s">
         <v>120</v>
       </c>
-      <c r="B13" s="94"/>
-      <c r="C13" s="95">
-        <v>556413.0</v>
-      </c>
-      <c r="D13" s="95">
+      <c r="B13" s="95"/>
+      <c r="C13" s="96">
+        <v>552721.0</v>
+      </c>
+      <c r="D13" s="96">
         <v>3420.0</v>
       </c>
-      <c r="E13" s="94">
-        <f t="shared" si="1"/>
-        <v>0.006146513471</v>
-      </c>
-      <c r="F13" s="94"/>
+      <c r="E13" s="95">
+        <f t="shared" si="1"/>
+        <v>0.006187570221</v>
+      </c>
+      <c r="F13" s="95"/>
     </row>
     <row r="14" ht="12.75" customHeight="1">
-      <c r="A14" s="93" t="s">
+      <c r="A14" s="94" t="s">
         <v>121</v>
       </c>
-      <c r="B14" s="94"/>
-      <c r="C14" s="95">
-        <v>885135.0</v>
-      </c>
-      <c r="D14" s="95">
+      <c r="B14" s="95"/>
+      <c r="C14" s="96">
+        <v>884377.0</v>
+      </c>
+      <c r="D14" s="96">
         <v>405726.0</v>
       </c>
-      <c r="E14" s="94">
-        <f t="shared" si="1"/>
-        <v>0.4583775356</v>
-      </c>
-      <c r="F14" s="94"/>
+      <c r="E14" s="95">
+        <f t="shared" si="1"/>
+        <v>0.4587704113</v>
+      </c>
+      <c r="F14" s="95"/>
     </row>
     <row r="15" ht="12.75" customHeight="1">
-      <c r="A15" s="96" t="s">
+      <c r="A15" s="97" t="s">
         <v>122</v>
       </c>
-      <c r="B15" s="94"/>
-      <c r="C15" s="95">
-        <v>1044608.0</v>
-      </c>
-      <c r="D15" s="95">
+      <c r="B15" s="95"/>
+      <c r="C15" s="96">
+        <v>1029679.0</v>
+      </c>
+      <c r="D15" s="96">
         <v>20983.0</v>
       </c>
-      <c r="E15" s="94">
-        <f t="shared" si="1"/>
-        <v>0.02008696085</v>
-      </c>
-      <c r="F15" s="94"/>
+      <c r="E15" s="95">
+        <f t="shared" si="1"/>
+        <v>0.02037819553</v>
+      </c>
+      <c r="F15" s="95"/>
     </row>
   </sheetData>
   <drawing r:id="rId1"/>
@@ -2963,7 +2964,7 @@
         <v>4</v>
       </c>
       <c r="B2" s="10">
-        <v>44308.0</v>
+        <v>44328.0</v>
       </c>
       <c r="C2" s="11" t="s">
         <v>5</v>
@@ -2971,7 +2972,7 @@
       <c r="D2" s="12">
         <v>44196.0</v>
       </c>
-      <c r="E2" s="86" t="s">
+      <c r="E2" s="87" t="s">
         <v>6</v>
       </c>
       <c r="F2" s="14" t="s">
@@ -2979,544 +2980,542 @@
       </c>
     </row>
     <row r="3" ht="12.75" customHeight="1">
-      <c r="A3" s="87"/>
-      <c r="B3" s="87"/>
-      <c r="C3" s="87"/>
-      <c r="D3" s="87"/>
-      <c r="E3" s="87"/>
-      <c r="F3" s="88" t="s">
+      <c r="A3" s="88"/>
+      <c r="B3" s="88"/>
+      <c r="C3" s="88"/>
+      <c r="D3" s="88"/>
+      <c r="E3" s="88"/>
+      <c r="F3" s="89" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="4" ht="13.5" customHeight="1">
-      <c r="A4" s="89" t="s">
+      <c r="A4" s="90" t="s">
         <v>9</v>
       </c>
-      <c r="B4" s="90" t="s">
+      <c r="B4" s="91" t="s">
         <v>105</v>
       </c>
-      <c r="C4" s="90" t="s">
+      <c r="C4" s="91"/>
+      <c r="D4" s="92"/>
+      <c r="E4" s="92"/>
+      <c r="F4" s="92"/>
+    </row>
+    <row r="5" ht="25.5" customHeight="1">
+      <c r="A5" s="93" t="s">
         <v>123</v>
       </c>
-      <c r="D4" s="91"/>
-      <c r="E4" s="91"/>
-      <c r="F4" s="91"/>
-    </row>
-    <row r="5" ht="25.5" customHeight="1">
-      <c r="A5" s="92" t="s">
+      <c r="B5" s="93" t="s">
+        <v>108</v>
+      </c>
+      <c r="C5" s="93" t="s">
+        <v>109</v>
+      </c>
+      <c r="D5" s="93" t="s">
+        <v>110</v>
+      </c>
+      <c r="E5" s="93" t="s">
+        <v>111</v>
+      </c>
+      <c r="F5" s="93" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="6" ht="12.75" customHeight="1">
+      <c r="A6" s="94" t="s">
         <v>124</v>
       </c>
-      <c r="B5" s="92" t="s">
-        <v>108</v>
-      </c>
-      <c r="C5" s="92" t="s">
-        <v>109</v>
-      </c>
-      <c r="D5" s="92" t="s">
-        <v>110</v>
-      </c>
-      <c r="E5" s="92" t="s">
-        <v>111</v>
-      </c>
-      <c r="F5" s="92" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="6" ht="12.75" customHeight="1">
-      <c r="A6" s="93" t="s">
+      <c r="B6" s="95"/>
+      <c r="C6" s="96">
+        <v>497114.0</v>
+      </c>
+      <c r="D6" s="96">
+        <v>502.0</v>
+      </c>
+      <c r="E6" s="98">
+        <f t="shared" ref="E6:E34" si="1">D6/C6</f>
+        <v>0.001009828731</v>
+      </c>
+      <c r="F6" s="95">
+        <f>E6-B6</f>
+        <v>0.001009828731</v>
+      </c>
+    </row>
+    <row r="7" ht="12.75" customHeight="1">
+      <c r="A7" s="94" t="s">
         <v>125</v>
       </c>
-      <c r="B6" s="94"/>
-      <c r="C6" s="95">
-        <v>590153.0</v>
-      </c>
-      <c r="D6" s="95">
-        <v>502.0</v>
-      </c>
-      <c r="E6" s="97">
-        <f t="shared" ref="E6:E34" si="1">D6/C6</f>
-        <v>0.0008506268713</v>
-      </c>
-      <c r="F6" s="94">
-        <f>E6-B6</f>
-        <v>0.0008506268713</v>
-      </c>
-    </row>
-    <row r="7" ht="12.75" customHeight="1">
-      <c r="A7" s="93" t="s">
+      <c r="B7" s="95"/>
+      <c r="C7" s="96">
+        <v>289943.0</v>
+      </c>
+      <c r="D7" s="96">
+        <v>18524.0</v>
+      </c>
+      <c r="E7" s="98">
+        <f t="shared" si="1"/>
+        <v>0.06388841945</v>
+      </c>
+      <c r="F7" s="95"/>
+    </row>
+    <row r="8" ht="12.75" customHeight="1">
+      <c r="A8" s="94" t="s">
         <v>126</v>
       </c>
-      <c r="B7" s="94"/>
-      <c r="C7" s="95">
-        <v>541510.0</v>
-      </c>
-      <c r="D7" s="95">
-        <v>24974.0</v>
-      </c>
-      <c r="E7" s="97">
-        <f t="shared" si="1"/>
-        <v>0.04611918524</v>
-      </c>
-      <c r="F7" s="94"/>
-    </row>
-    <row r="8" ht="12.75" customHeight="1">
-      <c r="A8" s="93" t="s">
+      <c r="B8" s="95"/>
+      <c r="C8" s="96">
+        <v>376294.0</v>
+      </c>
+      <c r="D8" s="96">
+        <v>0.0</v>
+      </c>
+      <c r="E8" s="98">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="F8" s="95"/>
+    </row>
+    <row r="9" ht="12.75" customHeight="1">
+      <c r="A9" s="94" t="s">
         <v>127</v>
       </c>
-      <c r="B8" s="94"/>
-      <c r="C8" s="95">
-        <v>376292.0</v>
-      </c>
-      <c r="D8" s="95">
+      <c r="B9" s="95"/>
+      <c r="C9" s="96">
+        <v>300241.0</v>
+      </c>
+      <c r="D9" s="96">
         <v>0.0</v>
       </c>
-      <c r="E8" s="97">
+      <c r="E9" s="98">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="F8" s="94"/>
-    </row>
-    <row r="9" ht="12.75" customHeight="1">
-      <c r="A9" s="93" t="s">
+      <c r="F9" s="95"/>
+    </row>
+    <row r="10" ht="12.75" customHeight="1">
+      <c r="A10" s="94" t="s">
         <v>128</v>
       </c>
-      <c r="B9" s="94"/>
-      <c r="C9" s="95">
-        <v>301134.0</v>
-      </c>
-      <c r="D9" s="95">
+      <c r="B10" s="95"/>
+      <c r="C10" s="96">
+        <v>164240.0</v>
+      </c>
+      <c r="D10" s="96">
+        <v>33288.0</v>
+      </c>
+      <c r="E10" s="98">
+        <f t="shared" si="1"/>
+        <v>0.2026790063</v>
+      </c>
+      <c r="F10" s="95"/>
+    </row>
+    <row r="11" ht="12.75" customHeight="1">
+      <c r="A11" s="94" t="s">
+        <v>129</v>
+      </c>
+      <c r="B11" s="95"/>
+      <c r="C11" s="96">
+        <v>325056.0</v>
+      </c>
+      <c r="D11" s="96">
+        <v>849.0</v>
+      </c>
+      <c r="E11" s="98">
+        <f t="shared" si="1"/>
+        <v>0.002611857649</v>
+      </c>
+      <c r="F11" s="95"/>
+    </row>
+    <row r="12" ht="12.75" customHeight="1">
+      <c r="A12" s="94" t="s">
+        <v>130</v>
+      </c>
+      <c r="B12" s="95"/>
+      <c r="C12" s="96">
+        <v>280286.0</v>
+      </c>
+      <c r="D12" s="96">
+        <v>73.0</v>
+      </c>
+      <c r="E12" s="98">
+        <f t="shared" si="1"/>
+        <v>0.0002604482564</v>
+      </c>
+      <c r="F12" s="95"/>
+    </row>
+    <row r="13" ht="12.75" customHeight="1">
+      <c r="A13" s="94" t="s">
+        <v>131</v>
+      </c>
+      <c r="B13" s="95"/>
+      <c r="C13" s="96">
+        <v>96222.0</v>
+      </c>
+      <c r="D13" s="96">
         <v>0.0</v>
       </c>
-      <c r="E9" s="97">
+      <c r="E13" s="98">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="F9" s="94"/>
-    </row>
-    <row r="10" ht="12.75" customHeight="1">
-      <c r="A10" s="93" t="s">
-        <v>129</v>
-      </c>
-      <c r="B10" s="94"/>
-      <c r="C10" s="95">
-        <v>164240.0</v>
-      </c>
-      <c r="D10" s="95">
-        <v>33288.0</v>
-      </c>
-      <c r="E10" s="97">
-        <f t="shared" si="1"/>
-        <v>0.2026790063</v>
-      </c>
-      <c r="F10" s="94"/>
-    </row>
-    <row r="11" ht="12.75" customHeight="1">
-      <c r="A11" s="93" t="s">
-        <v>130</v>
-      </c>
-      <c r="B11" s="94"/>
-      <c r="C11" s="95">
-        <v>339722.0</v>
-      </c>
-      <c r="D11" s="95">
-        <v>849.0</v>
-      </c>
-      <c r="E11" s="97">
-        <f t="shared" si="1"/>
-        <v>0.002499102207</v>
-      </c>
-      <c r="F11" s="94"/>
-    </row>
-    <row r="12" ht="12.75" customHeight="1">
-      <c r="A12" s="93" t="s">
-        <v>131</v>
-      </c>
-      <c r="B12" s="94"/>
-      <c r="C12" s="95">
-        <v>274532.0</v>
-      </c>
-      <c r="D12" s="95">
-        <v>73.0</v>
-      </c>
-      <c r="E12" s="97">
-        <f t="shared" si="1"/>
-        <v>0.0002659070709</v>
-      </c>
-      <c r="F12" s="94"/>
-    </row>
-    <row r="13" ht="12.75" customHeight="1">
-      <c r="A13" s="93" t="s">
+      <c r="F13" s="95"/>
+    </row>
+    <row r="14" ht="12.75" customHeight="1">
+      <c r="A14" s="94" t="s">
         <v>132</v>
       </c>
-      <c r="B13" s="94"/>
-      <c r="C13" s="95">
-        <v>96222.0</v>
-      </c>
-      <c r="D13" s="95">
+      <c r="B14" s="95"/>
+      <c r="C14" s="96">
+        <v>109883.0</v>
+      </c>
+      <c r="D14" s="96">
         <v>0.0</v>
       </c>
-      <c r="E13" s="97">
+      <c r="E14" s="98">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="F13" s="94"/>
-    </row>
-    <row r="14" ht="12.75" customHeight="1">
-      <c r="A14" s="93" t="s">
+      <c r="F14" s="95"/>
+    </row>
+    <row r="15" ht="12.75" customHeight="1">
+      <c r="A15" s="94" t="s">
         <v>133</v>
       </c>
-      <c r="B14" s="94"/>
-      <c r="C14" s="95">
-        <v>119061.0</v>
-      </c>
-      <c r="D14" s="95">
+      <c r="B15" s="95"/>
+      <c r="C15" s="96">
+        <v>1365393.0</v>
+      </c>
+      <c r="D15" s="96">
+        <v>829916.0</v>
+      </c>
+      <c r="E15" s="98">
+        <f t="shared" si="1"/>
+        <v>0.6078220703</v>
+      </c>
+      <c r="F15" s="95"/>
+    </row>
+    <row r="16" ht="12.75" customHeight="1">
+      <c r="A16" s="94" t="s">
+        <v>134</v>
+      </c>
+      <c r="B16" s="95"/>
+      <c r="C16" s="96">
+        <v>1367428.0</v>
+      </c>
+      <c r="D16" s="96">
+        <v>242701.0</v>
+      </c>
+      <c r="E16" s="98">
+        <f t="shared" si="1"/>
+        <v>0.1774872242</v>
+      </c>
+      <c r="F16" s="95"/>
+    </row>
+    <row r="17" ht="12.75" customHeight="1">
+      <c r="A17" s="94" t="s">
+        <v>135</v>
+      </c>
+      <c r="B17" s="95"/>
+      <c r="C17" s="96">
+        <v>382369.0</v>
+      </c>
+      <c r="D17" s="96">
+        <v>5900.0</v>
+      </c>
+      <c r="E17" s="98">
+        <f t="shared" si="1"/>
+        <v>0.01543012117</v>
+      </c>
+      <c r="F17" s="95"/>
+    </row>
+    <row r="18" ht="12.75" customHeight="1">
+      <c r="A18" s="94" t="s">
+        <v>136</v>
+      </c>
+      <c r="B18" s="95"/>
+      <c r="C18" s="96">
+        <v>379657.0</v>
+      </c>
+      <c r="D18" s="96">
         <v>0.0</v>
       </c>
-      <c r="E14" s="97">
+      <c r="E18" s="98">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="F14" s="94"/>
-    </row>
-    <row r="15" ht="12.75" customHeight="1">
-      <c r="A15" s="93" t="s">
-        <v>134</v>
-      </c>
-      <c r="B15" s="94"/>
-      <c r="C15" s="95">
-        <v>1389923.0</v>
-      </c>
-      <c r="D15" s="95">
-        <v>829916.0</v>
-      </c>
-      <c r="E15" s="97">
-        <f t="shared" si="1"/>
-        <v>0.597094947</v>
-      </c>
-      <c r="F15" s="94"/>
-    </row>
-    <row r="16" ht="12.75" customHeight="1">
-      <c r="A16" s="93" t="s">
-        <v>135</v>
-      </c>
-      <c r="B16" s="94"/>
-      <c r="C16" s="95">
-        <v>1479258.0</v>
-      </c>
-      <c r="D16" s="95">
-        <v>244555.0</v>
-      </c>
-      <c r="E16" s="97">
-        <f t="shared" si="1"/>
-        <v>0.1653227496</v>
-      </c>
-      <c r="F16" s="94"/>
-    </row>
-    <row r="17" ht="12.75" customHeight="1">
-      <c r="A17" s="93" t="s">
-        <v>136</v>
-      </c>
-      <c r="B17" s="94"/>
-      <c r="C17" s="95">
-        <v>382598.0</v>
-      </c>
-      <c r="D17" s="95">
-        <v>5900.0</v>
-      </c>
-      <c r="E17" s="97">
-        <f t="shared" si="1"/>
-        <v>0.01542088563</v>
-      </c>
-      <c r="F17" s="94"/>
-    </row>
-    <row r="18" ht="12.75" customHeight="1">
-      <c r="A18" s="93" t="s">
+      <c r="F18" s="95"/>
+    </row>
+    <row r="19" ht="12.75" customHeight="1">
+      <c r="A19" s="94" t="s">
         <v>137</v>
       </c>
-      <c r="B18" s="94"/>
-      <c r="C18" s="95">
-        <v>381341.0</v>
-      </c>
-      <c r="D18" s="95">
+      <c r="B19" s="95"/>
+      <c r="C19" s="96">
+        <v>263494.0</v>
+      </c>
+      <c r="D19" s="96">
         <v>0.0</v>
       </c>
-      <c r="E18" s="97">
+      <c r="E19" s="98">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="F18" s="94"/>
-    </row>
-    <row r="19" ht="12.75" customHeight="1">
-      <c r="A19" s="93" t="s">
+      <c r="F19" s="95"/>
+    </row>
+    <row r="20" ht="12.75" customHeight="1">
+      <c r="A20" s="94" t="s">
         <v>138</v>
       </c>
-      <c r="B19" s="94"/>
-      <c r="C19" s="95">
-        <v>225381.0</v>
-      </c>
-      <c r="D19" s="95">
+      <c r="B20" s="95"/>
+      <c r="C20" s="96">
+        <v>723363.0</v>
+      </c>
+      <c r="D20" s="96">
+        <v>5147.0</v>
+      </c>
+      <c r="E20" s="98">
+        <f t="shared" si="1"/>
+        <v>0.007115376374</v>
+      </c>
+      <c r="F20" s="95"/>
+    </row>
+    <row r="21" ht="12.75" customHeight="1">
+      <c r="A21" s="94" t="s">
+        <v>139</v>
+      </c>
+      <c r="B21" s="95"/>
+      <c r="C21" s="96">
+        <v>129383.0</v>
+      </c>
+      <c r="D21" s="96">
         <v>0.0</v>
       </c>
-      <c r="E19" s="97">
+      <c r="E21" s="98">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="F19" s="94"/>
-    </row>
-    <row r="20" ht="12.75" customHeight="1">
-      <c r="A20" s="93" t="s">
-        <v>139</v>
-      </c>
-      <c r="B20" s="94"/>
-      <c r="C20" s="95">
-        <v>781730.0</v>
-      </c>
-      <c r="D20" s="95">
-        <v>5147.0</v>
-      </c>
-      <c r="E20" s="97">
-        <f t="shared" si="1"/>
-        <v>0.00658411472</v>
-      </c>
-      <c r="F20" s="94"/>
-    </row>
-    <row r="21" ht="12.75" customHeight="1">
-      <c r="A21" s="93" t="s">
+      <c r="F21" s="95"/>
+    </row>
+    <row r="22" ht="12.75" customHeight="1">
+      <c r="A22" s="94" t="s">
         <v>140</v>
       </c>
-      <c r="B21" s="94"/>
-      <c r="C21" s="95">
-        <v>128922.0</v>
-      </c>
-      <c r="D21" s="95">
+      <c r="B22" s="95"/>
+      <c r="C22" s="96">
+        <v>123280.0</v>
+      </c>
+      <c r="D22" s="96">
         <v>0.0</v>
       </c>
-      <c r="E21" s="97">
+      <c r="E22" s="98">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="F21" s="94"/>
-    </row>
-    <row r="22" ht="12.75" customHeight="1">
-      <c r="A22" s="93" t="s">
+      <c r="F22" s="95"/>
+    </row>
+    <row r="23" ht="12.75" customHeight="1">
+      <c r="A23" s="94" t="s">
         <v>141</v>
       </c>
-      <c r="B22" s="94"/>
-      <c r="C22" s="95">
-        <v>138507.0</v>
-      </c>
-      <c r="D22" s="95">
+      <c r="B23" s="95"/>
+      <c r="C23" s="96">
+        <v>56621.0</v>
+      </c>
+      <c r="D23" s="96">
         <v>0.0</v>
       </c>
-      <c r="E22" s="97">
+      <c r="E23" s="98">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="F22" s="94"/>
-    </row>
-    <row r="23" ht="12.75" customHeight="1">
-      <c r="A23" s="93" t="s">
+      <c r="F23" s="95"/>
+    </row>
+    <row r="24" ht="12.75" customHeight="1">
+      <c r="A24" s="94" t="s">
         <v>142</v>
       </c>
-      <c r="B23" s="94"/>
-      <c r="C23" s="95">
-        <v>56051.0</v>
-      </c>
-      <c r="D23" s="95">
+      <c r="B24" s="95"/>
+      <c r="C24" s="96">
+        <v>296646.0</v>
+      </c>
+      <c r="D24" s="96">
+        <v>2497.0</v>
+      </c>
+      <c r="E24" s="98">
+        <f t="shared" si="1"/>
+        <v>0.008417440316</v>
+      </c>
+      <c r="F24" s="95"/>
+    </row>
+    <row r="25" ht="12.75" customHeight="1">
+      <c r="A25" s="94" t="s">
+        <v>143</v>
+      </c>
+      <c r="B25" s="95"/>
+      <c r="C25" s="96">
+        <v>347442.0</v>
+      </c>
+      <c r="D25" s="96">
+        <v>3420.0</v>
+      </c>
+      <c r="E25" s="98">
+        <f t="shared" si="1"/>
+        <v>0.009843369541</v>
+      </c>
+      <c r="F25" s="95"/>
+    </row>
+    <row r="26" ht="12.75" customHeight="1">
+      <c r="A26" s="94" t="s">
+        <v>144</v>
+      </c>
+      <c r="B26" s="95"/>
+      <c r="C26" s="96">
+        <v>365056.0</v>
+      </c>
+      <c r="D26" s="96">
+        <v>1404.0</v>
+      </c>
+      <c r="E26" s="98">
+        <f t="shared" si="1"/>
+        <v>0.003845985273</v>
+      </c>
+      <c r="F26" s="95"/>
+    </row>
+    <row r="27" ht="12.75" customHeight="1">
+      <c r="A27" s="94" t="s">
+        <v>145</v>
+      </c>
+      <c r="B27" s="95"/>
+      <c r="C27" s="96">
+        <v>310415.0</v>
+      </c>
+      <c r="D27" s="96">
+        <v>67495.0</v>
+      </c>
+      <c r="E27" s="98">
+        <f t="shared" si="1"/>
+        <v>0.2174347245</v>
+      </c>
+      <c r="F27" s="95"/>
+    </row>
+    <row r="28" ht="12.75" customHeight="1">
+      <c r="A28" s="94" t="s">
+        <v>146</v>
+      </c>
+      <c r="B28" s="95"/>
+      <c r="C28" s="96">
+        <v>320082.0</v>
+      </c>
+      <c r="D28" s="96">
         <v>0.0</v>
       </c>
-      <c r="E23" s="97">
+      <c r="E28" s="98">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="F23" s="94"/>
-    </row>
-    <row r="24" ht="12.75" customHeight="1">
-      <c r="A24" s="93" t="s">
-        <v>143</v>
-      </c>
-      <c r="B24" s="94"/>
-      <c r="C24" s="95">
-        <v>595874.0</v>
-      </c>
-      <c r="D24" s="95">
-        <v>5032.0</v>
-      </c>
-      <c r="E24" s="97">
-        <f t="shared" si="1"/>
-        <v>0.008444738317</v>
-      </c>
-      <c r="F24" s="94"/>
-    </row>
-    <row r="25" ht="12.75" customHeight="1">
-      <c r="A25" s="93" t="s">
-        <v>144</v>
-      </c>
-      <c r="B25" s="94"/>
-      <c r="C25" s="95">
-        <v>346312.0</v>
-      </c>
-      <c r="D25" s="95">
-        <v>3420.0</v>
-      </c>
-      <c r="E25" s="97">
-        <f t="shared" si="1"/>
-        <v>0.009875487999</v>
-      </c>
-      <c r="F25" s="94"/>
-    </row>
-    <row r="26" ht="12.75" customHeight="1">
-      <c r="A26" s="93" t="s">
-        <v>145</v>
-      </c>
-      <c r="B26" s="94"/>
-      <c r="C26" s="95">
-        <v>376969.0</v>
-      </c>
-      <c r="D26" s="95">
-        <v>1404.0</v>
-      </c>
-      <c r="E26" s="97">
-        <f t="shared" si="1"/>
-        <v>0.003724444185</v>
-      </c>
-      <c r="F26" s="94"/>
-    </row>
-    <row r="27" ht="12.75" customHeight="1">
-      <c r="A27" s="93" t="s">
-        <v>146</v>
-      </c>
-      <c r="B27" s="94"/>
-      <c r="C27" s="95">
-        <v>310777.0</v>
-      </c>
-      <c r="D27" s="95">
-        <v>67495.0</v>
-      </c>
-      <c r="E27" s="97">
-        <f t="shared" si="1"/>
-        <v>0.2171814517</v>
-      </c>
-      <c r="F27" s="94"/>
-    </row>
-    <row r="28" ht="12.75" customHeight="1">
-      <c r="A28" s="93" t="s">
+      <c r="F28" s="95"/>
+    </row>
+    <row r="29" ht="12.75" customHeight="1">
+      <c r="A29" s="94" t="s">
         <v>147</v>
       </c>
-      <c r="B28" s="94"/>
-      <c r="C28" s="95">
-        <v>320085.0</v>
-      </c>
-      <c r="D28" s="95">
+      <c r="B29" s="95"/>
+      <c r="C29" s="96">
+        <v>200778.0</v>
+      </c>
+      <c r="D29" s="96">
         <v>0.0</v>
       </c>
-      <c r="E28" s="97">
+      <c r="E29" s="98">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="F28" s="94"/>
-    </row>
-    <row r="29" ht="12.75" customHeight="1">
-      <c r="A29" s="93" t="s">
+      <c r="F29" s="95"/>
+    </row>
+    <row r="30" ht="12.75" customHeight="1">
+      <c r="A30" s="94" t="s">
         <v>148</v>
       </c>
-      <c r="B29" s="94"/>
-      <c r="C29" s="95">
-        <v>200804.0</v>
-      </c>
-      <c r="D29" s="95">
-        <v>0.0</v>
-      </c>
-      <c r="E29" s="97">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="F29" s="94"/>
-    </row>
-    <row r="30" ht="12.75" customHeight="1">
-      <c r="A30" s="93" t="s">
+      <c r="B30" s="95"/>
+      <c r="C30" s="96">
+        <v>152565.0</v>
+      </c>
+      <c r="D30" s="96">
+        <v>188.0</v>
+      </c>
+      <c r="E30" s="98">
+        <f t="shared" si="1"/>
+        <v>0.001232261659</v>
+      </c>
+      <c r="F30" s="95"/>
+    </row>
+    <row r="31" ht="12.75" customHeight="1">
+      <c r="A31" s="94" t="s">
         <v>149</v>
       </c>
-      <c r="B30" s="94"/>
-      <c r="C30" s="95">
-        <v>195300.0</v>
-      </c>
-      <c r="D30" s="95">
-        <v>188.0</v>
-      </c>
-      <c r="E30" s="97">
-        <f t="shared" si="1"/>
-        <v>0.0009626216078</v>
-      </c>
-      <c r="F30" s="94"/>
-    </row>
-    <row r="31" ht="12.75" customHeight="1">
-      <c r="A31" s="93" t="s">
+      <c r="B31" s="95"/>
+      <c r="C31" s="96">
+        <v>852822.0</v>
+      </c>
+      <c r="D31" s="96">
+        <v>338231.0</v>
+      </c>
+      <c r="E31" s="98">
+        <f t="shared" si="1"/>
+        <v>0.3966021045</v>
+      </c>
+      <c r="F31" s="95"/>
+    </row>
+    <row r="32" ht="12.75" customHeight="1">
+      <c r="A32" s="94" t="s">
         <v>150</v>
       </c>
-      <c r="B31" s="94"/>
-      <c r="C31" s="95">
-        <v>853599.0</v>
-      </c>
-      <c r="D31" s="95">
-        <v>338231.0</v>
-      </c>
-      <c r="E31" s="97">
-        <f t="shared" si="1"/>
-        <v>0.3962410921</v>
-      </c>
-      <c r="F31" s="94"/>
-    </row>
-    <row r="32" ht="12.75" customHeight="1">
-      <c r="A32" s="93" t="s">
+      <c r="B32" s="95"/>
+      <c r="C32" s="96">
+        <v>328618.0</v>
+      </c>
+      <c r="D32" s="96">
+        <v>2607.0</v>
+      </c>
+      <c r="E32" s="98">
+        <f t="shared" si="1"/>
+        <v>0.007933223378</v>
+      </c>
+      <c r="F32" s="95"/>
+    </row>
+    <row r="33" ht="12.75" customHeight="1">
+      <c r="A33" s="94" t="s">
         <v>151</v>
       </c>
-      <c r="B32" s="94"/>
-      <c r="C32" s="95">
-        <v>351196.0</v>
-      </c>
-      <c r="D32" s="95">
-        <v>2607.0</v>
-      </c>
-      <c r="E32" s="97">
-        <f t="shared" si="1"/>
-        <v>0.007423205276</v>
-      </c>
-      <c r="F32" s="94"/>
-    </row>
-    <row r="33" ht="12.75" customHeight="1">
-      <c r="A33" s="93" t="s">
+      <c r="B33" s="95"/>
+      <c r="C33" s="96">
+        <v>535153.0</v>
+      </c>
+      <c r="D33" s="96">
+        <v>19303.0</v>
+      </c>
+      <c r="E33" s="98">
+        <f t="shared" si="1"/>
+        <v>0.03607005847</v>
+      </c>
+      <c r="F33" s="95"/>
+    </row>
+    <row r="34" ht="12.75" customHeight="1">
+      <c r="A34" s="94" t="s">
         <v>152</v>
       </c>
-      <c r="B33" s="94"/>
-      <c r="C33" s="95">
-        <v>477046.0</v>
-      </c>
-      <c r="D33" s="95">
-        <v>19303.0</v>
-      </c>
-      <c r="E33" s="97">
-        <f t="shared" si="1"/>
-        <v>0.04046360309</v>
-      </c>
-      <c r="F33" s="94"/>
-    </row>
-    <row r="34" ht="12.75" customHeight="1">
-      <c r="A34" s="93" t="s">
-        <v>153</v>
-      </c>
-      <c r="B34" s="94"/>
-      <c r="C34" s="95">
-        <v>1062413.0</v>
-      </c>
-      <c r="D34" s="95">
-        <v>21094.0</v>
-      </c>
-      <c r="E34" s="97">
-        <f t="shared" si="1"/>
-        <v>0.01985480223</v>
-      </c>
-      <c r="F34" s="94"/>
+      <c r="B34" s="95"/>
+      <c r="C34" s="96">
+        <v>1004515.0</v>
+      </c>
+      <c r="D34" s="96">
+        <v>20983.0</v>
+      </c>
+      <c r="E34" s="98">
+        <f t="shared" si="1"/>
+        <v>0.02088868758</v>
+      </c>
+      <c r="F34" s="95"/>
     </row>
   </sheetData>
   <drawing r:id="rId1"/>
@@ -3540,50 +3539,58 @@
   </cols>
   <sheetData>
     <row r="1" ht="12.0" customHeight="1">
-      <c r="A1" s="98" t="s">
+      <c r="A1" s="99" t="s">
+        <v>153</v>
+      </c>
+      <c r="B1" s="99" t="s">
+        <v>123</v>
+      </c>
+      <c r="C1" s="99" t="s">
         <v>154</v>
       </c>
-      <c r="B1" s="98" t="s">
+      <c r="D1" s="99" t="s">
         <v>155</v>
       </c>
-      <c r="C1" s="98" t="s">
+    </row>
+    <row r="2" ht="15.75" customHeight="1">
+      <c r="A2" s="100">
+        <v>44308.0</v>
+      </c>
+      <c r="B2" s="101" t="s">
         <v>156</v>
       </c>
-      <c r="D1" s="98" t="s">
+      <c r="C2" s="102">
+        <v>2020.0</v>
+      </c>
+      <c r="D2" s="101" t="s">
         <v>157</v>
       </c>
     </row>
-    <row r="2" ht="15.75" customHeight="1">
-      <c r="A2" s="99">
-        <v>44308.0</v>
-      </c>
-      <c r="B2" s="100" t="s">
+    <row r="3" ht="15.75" customHeight="1">
+      <c r="A3" s="100">
+        <v>44328.0</v>
+      </c>
+      <c r="B3" s="101" t="s">
+        <v>156</v>
+      </c>
+      <c r="C3" s="102">
+        <v>2020.0</v>
+      </c>
+      <c r="D3" s="101" t="s">
         <v>158</v>
       </c>
-      <c r="C2" s="101">
-        <v>2020.0</v>
-      </c>
-      <c r="D2" s="100" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="3" ht="15.75" customHeight="1">
-      <c r="A3" s="102"/>
-      <c r="B3" s="100"/>
-      <c r="C3" s="103"/>
-      <c r="D3" s="100"/>
     </row>
     <row r="4" ht="15.75" customHeight="1">
-      <c r="A4" s="102"/>
-      <c r="B4" s="100"/>
+      <c r="A4" s="103"/>
+      <c r="B4" s="101"/>
       <c r="C4" s="104"/>
-      <c r="D4" s="100"/>
+      <c r="D4" s="101"/>
     </row>
     <row r="5" ht="15.75" customHeight="1">
-      <c r="A5" s="99"/>
+      <c r="A5" s="100"/>
       <c r="B5" s="105"/>
-      <c r="C5" s="103"/>
-      <c r="D5" s="106"/>
+      <c r="C5" s="106"/>
+      <c r="D5" s="107"/>
     </row>
   </sheetData>
   <drawing r:id="rId1"/>

</xml_diff>

<commit_message>
UK removed in RP3
</commit_message>
<xml_diff>
--- a/static/download/2020/RP3_ERT_ATFM_2020_Jan_Dec.xlsx
+++ b/static/download/2020/RP3_ERT_ATFM_2020_Jan_Dec.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="215" uniqueCount="159">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="218" uniqueCount="161">
   <si>
     <t>Data source</t>
   </si>
@@ -47,7 +47,7 @@
     <t>Period: JAN-DEC</t>
   </si>
   <si>
-    <t>SES Area</t>
+    <t>SES Area (RP3)</t>
   </si>
   <si>
     <t>Area</t>
@@ -74,7 +74,7 @@
     <t>% of flights with en-route ATFM delay greater than 15 min</t>
   </si>
   <si>
-    <t>SES area</t>
+    <t>SES area (RP3)</t>
   </si>
   <si>
     <t xml:space="preserve">2015 </t>
@@ -389,93 +389,93 @@
     <t>Entity</t>
   </si>
   <si>
+    <t>ANS CR</t>
+  </si>
+  <si>
     <t>Austro Control</t>
   </si>
   <si>
+    <t>Avinor</t>
+  </si>
+  <si>
+    <t>BULATSA</t>
+  </si>
+  <si>
+    <t>Croatia Control</t>
+  </si>
+  <si>
+    <t>DCAC Cyprus</t>
+  </si>
+  <si>
+    <t>DFS</t>
+  </si>
+  <si>
+    <t>DSNA</t>
+  </si>
+  <si>
+    <t>EANS</t>
+  </si>
+  <si>
+    <t>ENAIRE</t>
+  </si>
+  <si>
+    <t>ENAV</t>
+  </si>
+  <si>
+    <t>Fintraffic ANS</t>
+  </si>
+  <si>
+    <t>HCAA</t>
+  </si>
+  <si>
+    <t>HungaroControl (EC)</t>
+  </si>
+  <si>
+    <t>IAA</t>
+  </si>
+  <si>
+    <t>LFV</t>
+  </si>
+  <si>
+    <t>LGS</t>
+  </si>
+  <si>
+    <t>LPS</t>
+  </si>
+  <si>
+    <t>LVNL</t>
+  </si>
+  <si>
+    <t>Maastricht UAC</t>
+  </si>
+  <si>
+    <t>MATS</t>
+  </si>
+  <si>
+    <t>NAV Portugal</t>
+  </si>
+  <si>
+    <t>NAVIAIR</t>
+  </si>
+  <si>
+    <t>Oro navigacija</t>
+  </si>
+  <si>
+    <t>PANSA</t>
+  </si>
+  <si>
+    <t>ROMATSA</t>
+  </si>
+  <si>
     <t>skeyes</t>
   </si>
   <si>
-    <t>BULATSA</t>
-  </si>
-  <si>
-    <t>Croatia Control</t>
-  </si>
-  <si>
-    <t>DCAC Cyprus</t>
-  </si>
-  <si>
-    <t>ANS CR</t>
-  </si>
-  <si>
-    <t>NAVIAIR</t>
-  </si>
-  <si>
-    <t>EANS</t>
-  </si>
-  <si>
-    <t>Fintraffic ANS</t>
-  </si>
-  <si>
-    <t>DSNA</t>
-  </si>
-  <si>
-    <t>DFS</t>
-  </si>
-  <si>
-    <t>HCAA</t>
-  </si>
-  <si>
-    <t>HungaroControl (EC)</t>
-  </si>
-  <si>
-    <t>IAA</t>
-  </si>
-  <si>
-    <t>ENAV</t>
-  </si>
-  <si>
-    <t>LGS</t>
-  </si>
-  <si>
-    <t>Oro navigacija</t>
-  </si>
-  <si>
-    <t>MATS</t>
-  </si>
-  <si>
-    <t>LVNL</t>
-  </si>
-  <si>
-    <t>Avinor</t>
-  </si>
-  <si>
-    <t>PANSA</t>
-  </si>
-  <si>
-    <t>NAV Portugal</t>
-  </si>
-  <si>
-    <t>ROMATSA</t>
-  </si>
-  <si>
-    <t>LPS</t>
+    <t>Skyguide</t>
   </si>
   <si>
     <t>Slovenia Control</t>
   </si>
   <si>
-    <t>ENAIRE</t>
-  </si>
-  <si>
-    <t>LFV</t>
-  </si>
-  <si>
-    <t>Skyguide</t>
-  </si>
-  <si>
-    <t>NATS (Continental)</t>
-  </si>
-  <si>
     <t>Change date</t>
   </si>
   <si>
@@ -492,6 +492,12 @@
   </si>
   <si>
     <t>Local level changed to ANSP</t>
+  </si>
+  <si>
+    <t>UK</t>
+  </si>
+  <si>
+    <t>UK removed</t>
   </si>
 </sst>
 </file>
@@ -847,7 +853,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="108">
+  <cellXfs count="107">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -1152,9 +1158,6 @@
     </xf>
     <xf borderId="0" fillId="3" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="0" fillId="3" fontId="10" numFmtId="164" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
-      <alignment horizontal="center" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="10" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0" shrinkToFit="0" wrapText="0"/>
@@ -1244,7 +1247,7 @@
         <v>4</v>
       </c>
       <c r="B2" s="10">
-        <v>44308.0</v>
+        <v>44351.0</v>
       </c>
       <c r="C2" s="11" t="s">
         <v>5</v>
@@ -1330,21 +1333,21 @@
       </c>
       <c r="C6" s="31">
         <f t="shared" ref="C6:C11" si="1">E6/D6</f>
-        <v>0.7608276904</v>
+        <v>0.7757046325</v>
       </c>
       <c r="D6" s="32">
-        <v>9242345.0</v>
+        <v>8820414.0</v>
       </c>
       <c r="E6" s="33">
-        <v>7031832.0</v>
+        <v>6842036.0</v>
       </c>
       <c r="F6" s="34"/>
       <c r="G6" s="35">
         <f t="shared" ref="G6:G11" si="2">C6-F6</f>
-        <v>0.7608276904</v>
+        <v>0.7757046325</v>
       </c>
       <c r="H6" s="36">
-        <v>0.019</v>
+        <v>0.0193</v>
       </c>
     </row>
     <row r="7" ht="12.0" customHeight="1">
@@ -1356,21 +1359,21 @@
       </c>
       <c r="C7" s="31">
         <f t="shared" si="1"/>
-        <v>0.9143127931</v>
+        <v>0.8742416857</v>
       </c>
       <c r="D7" s="38">
-        <v>9505573.0</v>
+        <v>9086437.0</v>
       </c>
       <c r="E7" s="39">
-        <v>8691067.0</v>
+        <v>7943742.0</v>
       </c>
       <c r="F7" s="40"/>
       <c r="G7" s="41">
         <f t="shared" si="2"/>
-        <v>0.9143127931</v>
+        <v>0.8742416857</v>
       </c>
       <c r="H7" s="36">
-        <v>0.0217</v>
+        <v>0.0206</v>
       </c>
     </row>
     <row r="8" ht="12.0" customHeight="1">
@@ -1382,21 +1385,21 @@
       </c>
       <c r="C8" s="31">
         <f t="shared" si="1"/>
-        <v>0.941046466</v>
+        <v>0.938859843</v>
       </c>
       <c r="D8" s="38">
-        <v>9847620.0</v>
+        <v>9425491.0</v>
       </c>
       <c r="E8" s="39">
-        <v>9267068.0</v>
+        <v>8849215.0</v>
       </c>
       <c r="F8" s="34"/>
       <c r="G8" s="41">
         <f t="shared" si="2"/>
-        <v>0.941046466</v>
+        <v>0.938859843</v>
       </c>
       <c r="H8" s="36">
-        <v>0.0218</v>
+        <v>0.0217</v>
       </c>
     </row>
     <row r="9" ht="12.0" customHeight="1">
@@ -1408,21 +1411,21 @@
       </c>
       <c r="C9" s="31">
         <f t="shared" si="1"/>
-        <v>1.827205784</v>
+        <v>1.830159819</v>
       </c>
       <c r="D9" s="38">
-        <v>1.0215122E7</v>
+        <v>9800596.0</v>
       </c>
       <c r="E9" s="39">
-        <v>1.866513E7</v>
+        <v>1.7936657E7</v>
       </c>
       <c r="F9" s="34"/>
       <c r="G9" s="41">
         <f t="shared" si="2"/>
-        <v>1.827205784</v>
+        <v>1.830159819</v>
       </c>
       <c r="H9" s="36">
-        <v>0.0437</v>
+        <v>0.0438</v>
       </c>
     </row>
     <row r="10" ht="12.0" customHeight="1">
@@ -1434,21 +1437,21 @@
       </c>
       <c r="C10" s="31">
         <f t="shared" si="1"/>
-        <v>1.666567384</v>
+        <v>1.679992502</v>
       </c>
       <c r="D10" s="38">
-        <v>1.0334109E7</v>
+        <v>9933936.0</v>
       </c>
       <c r="E10" s="39">
-        <v>1.7222489E7</v>
+        <v>1.6688938E7</v>
       </c>
       <c r="F10" s="34"/>
       <c r="G10" s="41">
         <f t="shared" si="2"/>
-        <v>1.666567384</v>
+        <v>1.679992502</v>
       </c>
       <c r="H10" s="36">
-        <v>0.0391</v>
+        <v>0.0394</v>
       </c>
     </row>
     <row r="11" ht="12.0" customHeight="1">
@@ -1460,23 +1463,23 @@
       </c>
       <c r="C11" s="31">
         <f t="shared" si="1"/>
-        <v>0.348000394</v>
+        <v>0.3570113323</v>
       </c>
       <c r="D11" s="38">
-        <v>4608808.0</v>
+        <v>4433708.0</v>
       </c>
       <c r="E11" s="39">
-        <v>1603867.0</v>
+        <v>1582884.0</v>
       </c>
       <c r="F11" s="42">
         <v>0.9</v>
       </c>
       <c r="G11" s="41">
         <f t="shared" si="2"/>
-        <v>-0.551999606</v>
+        <v>-0.5429886677</v>
       </c>
       <c r="H11" s="36">
-        <v>0.0071</v>
+        <v>0.0072</v>
       </c>
     </row>
     <row r="12" ht="12.0" customHeight="1">
@@ -1597,7 +1600,7 @@
         <v>4</v>
       </c>
       <c r="B2" s="10">
-        <v>44308.0</v>
+        <v>44351.0</v>
       </c>
       <c r="C2" s="11" t="s">
         <v>5</v>
@@ -1662,13 +1665,13 @@
       </c>
       <c r="B6" s="62">
         <f t="shared" ref="B6:B29" si="1">D6/C6</f>
-        <v>0.3881771646</v>
+        <v>0.4041344334</v>
       </c>
       <c r="C6" s="63">
-        <v>730620.0</v>
+        <v>699975.0</v>
       </c>
       <c r="D6" s="64">
-        <v>283610.0</v>
+        <v>282884.0</v>
       </c>
       <c r="E6" s="65"/>
       <c r="F6" s="66">
@@ -1681,13 +1684,13 @@
       </c>
       <c r="B7" s="67">
         <f t="shared" si="1"/>
-        <v>0.4865745041</v>
+        <v>0.4933644225</v>
       </c>
       <c r="C7" s="68">
-        <v>686902.0</v>
+        <v>657893.0</v>
       </c>
       <c r="D7" s="69">
-        <v>334229.0</v>
+        <v>324581.0</v>
       </c>
       <c r="E7" s="65"/>
       <c r="F7" s="66">
@@ -1700,13 +1703,13 @@
       </c>
       <c r="B8" s="67">
         <f t="shared" si="1"/>
-        <v>0.9718605532</v>
+        <v>1.012783337</v>
       </c>
       <c r="C8" s="68">
-        <v>786938.0</v>
+        <v>753872.0</v>
       </c>
       <c r="D8" s="69">
-        <v>764794.0</v>
+        <v>763509.0</v>
       </c>
       <c r="E8" s="65"/>
       <c r="F8" s="66">
@@ -1719,13 +1722,13 @@
       </c>
       <c r="B9" s="67">
         <f t="shared" si="1"/>
-        <v>1.133095043</v>
+        <v>1.148831511</v>
       </c>
       <c r="C9" s="69">
-        <v>848544.0</v>
+        <v>815412.0</v>
       </c>
       <c r="D9" s="69">
-        <v>961481.0</v>
+        <v>936771.0</v>
       </c>
       <c r="E9" s="65"/>
       <c r="F9" s="66">
@@ -1738,13 +1741,13 @@
       </c>
       <c r="B10" s="67">
         <f t="shared" si="1"/>
-        <v>1.858407406</v>
+        <v>1.914318462</v>
       </c>
       <c r="C10" s="69">
-        <v>921729.0</v>
+        <v>886422.0</v>
       </c>
       <c r="D10" s="69">
-        <v>1712948.0</v>
+        <v>1696894.0</v>
       </c>
       <c r="E10" s="65"/>
       <c r="F10" s="66">
@@ -1757,13 +1760,13 @@
       </c>
       <c r="B11" s="67">
         <f t="shared" si="1"/>
-        <v>2.957661543</v>
+        <v>2.988936024</v>
       </c>
       <c r="C11" s="69">
-        <v>966757.0</v>
+        <v>932305.0</v>
       </c>
       <c r="D11" s="69">
-        <v>2859340.0</v>
+        <v>2786600.0</v>
       </c>
       <c r="E11" s="65"/>
       <c r="F11" s="66">
@@ -1776,13 +1779,13 @@
       </c>
       <c r="B12" s="67">
         <f t="shared" si="1"/>
-        <v>3.379891483</v>
+        <v>3.369078543</v>
       </c>
       <c r="C12" s="69">
-        <v>1018454.0</v>
+        <v>982444.0</v>
       </c>
       <c r="D12" s="69">
-        <v>3442264.0</v>
+        <v>3309931.0</v>
       </c>
       <c r="E12" s="70" t="s">
         <v>8</v>
@@ -1797,13 +1800,13 @@
       </c>
       <c r="B13" s="67">
         <f t="shared" si="1"/>
-        <v>2.844248328</v>
+        <v>2.808366039</v>
       </c>
       <c r="C13" s="69">
-        <v>1005864.0</v>
+        <v>970256.0</v>
       </c>
       <c r="D13" s="69">
-        <v>2860927.0</v>
+        <v>2724834.0</v>
       </c>
       <c r="E13" s="65"/>
       <c r="F13" s="66">
@@ -1816,13 +1819,13 @@
       </c>
       <c r="B14" s="67">
         <f t="shared" si="1"/>
-        <v>1.905906347</v>
+        <v>1.895806678</v>
       </c>
       <c r="C14" s="69">
-        <v>966909.0</v>
+        <v>932411.0</v>
       </c>
       <c r="D14" s="69">
-        <v>1842838.0</v>
+        <v>1767671.0</v>
       </c>
       <c r="E14" s="65"/>
       <c r="F14" s="66">
@@ -1835,13 +1838,13 @@
       </c>
       <c r="B15" s="67">
         <f t="shared" si="1"/>
-        <v>1.063593354</v>
+        <v>1.049598995</v>
       </c>
       <c r="C15" s="69">
-        <v>915646.0</v>
+        <v>880038.0</v>
       </c>
       <c r="D15" s="69">
-        <v>973875.0</v>
+        <v>923687.0</v>
       </c>
       <c r="E15" s="65"/>
       <c r="F15" s="66">
@@ -1854,13 +1857,13 @@
       </c>
       <c r="B16" s="67">
         <f t="shared" si="1"/>
-        <v>0.3414012739</v>
+        <v>0.3515899995</v>
       </c>
       <c r="C16" s="69">
-        <v>745750.0</v>
+        <v>713365.0</v>
       </c>
       <c r="D16" s="69">
-        <v>254600.0</v>
+        <v>250812.0</v>
       </c>
       <c r="E16" s="65"/>
       <c r="F16" s="66">
@@ -1873,13 +1876,13 @@
       </c>
       <c r="B17" s="71">
         <f t="shared" si="1"/>
-        <v>1.258902751</v>
+        <v>1.297685975</v>
       </c>
       <c r="C17" s="72">
-        <v>739996.0</v>
+        <v>709543.0</v>
       </c>
       <c r="D17" s="72">
-        <v>931583.0</v>
+        <v>920764.0</v>
       </c>
       <c r="E17" s="73"/>
       <c r="F17" s="66">
@@ -1892,17 +1895,17 @@
       </c>
       <c r="B18" s="62">
         <f t="shared" si="1"/>
-        <v>0.5024975326</v>
+        <v>0.5179546649</v>
       </c>
       <c r="C18" s="64">
-        <v>729520.0</v>
+        <v>700208.0</v>
       </c>
       <c r="D18" s="64">
-        <v>366582.0</v>
+        <v>362676.0</v>
       </c>
       <c r="E18" s="74">
         <f>D18/C18</f>
-        <v>0.5024975326</v>
+        <v>0.5179546649</v>
       </c>
       <c r="F18" s="75">
         <v>1.0</v>
@@ -1914,17 +1917,17 @@
       </c>
       <c r="B19" s="67">
         <f t="shared" si="1"/>
-        <v>0.8431746872</v>
+        <v>0.8578355891</v>
       </c>
       <c r="C19" s="69">
-        <v>695111.0</v>
+        <v>666306.0</v>
       </c>
       <c r="D19" s="69">
-        <v>586100.0</v>
+        <v>571581.0</v>
       </c>
       <c r="E19" s="67">
         <f t="shared" ref="E19:E29" si="2">sum(D$18:D19)/sum(C$18:C19)</f>
-        <v>0.6687219357</v>
+        <v>0.6836790549</v>
       </c>
       <c r="F19" s="76">
         <v>1.0</v>
@@ -1936,17 +1939,17 @@
       </c>
       <c r="B20" s="67">
         <f t="shared" si="1"/>
-        <v>1.318724928</v>
+        <v>1.374425536</v>
       </c>
       <c r="C20" s="69">
-        <v>463660.0</v>
+        <v>443239.0</v>
       </c>
       <c r="D20" s="69">
-        <v>611440.0</v>
+        <v>609199.0</v>
       </c>
       <c r="E20" s="67">
         <f t="shared" si="2"/>
-        <v>0.828326778</v>
+        <v>0.8528545056</v>
       </c>
       <c r="F20" s="76">
         <v>1.0</v>
@@ -1958,17 +1961,17 @@
       </c>
       <c r="B21" s="67">
         <f t="shared" si="1"/>
-        <v>0.001483809025</v>
+        <v>0.001553583396</v>
       </c>
       <c r="C21" s="69">
-        <v>103113.0</v>
+        <v>98482.0</v>
       </c>
       <c r="D21" s="69">
         <v>153.0</v>
       </c>
       <c r="E21" s="67">
         <f t="shared" si="2"/>
-        <v>0.7855136376</v>
+        <v>0.8089197609</v>
       </c>
       <c r="F21" s="76">
         <v>1.0</v>
@@ -1980,17 +1983,17 @@
       </c>
       <c r="B22" s="67">
         <f t="shared" si="1"/>
-        <v>0.02324166829</v>
+        <v>0.02419386359</v>
       </c>
       <c r="C22" s="69">
-        <v>133166.0</v>
+        <v>127925.0</v>
       </c>
       <c r="D22" s="69">
         <v>3095.0</v>
       </c>
       <c r="E22" s="67">
         <f t="shared" si="2"/>
-        <v>0.7377351652</v>
+        <v>0.7596181047</v>
       </c>
       <c r="F22" s="76">
         <v>1.0</v>
@@ -2002,17 +2005,17 @@
       </c>
       <c r="B23" s="67">
         <f t="shared" si="1"/>
-        <v>0.01531771176</v>
+        <v>0.01580281065</v>
       </c>
       <c r="C23" s="69">
-        <v>200748.0</v>
+        <v>193763.0</v>
       </c>
       <c r="D23" s="69">
-        <v>3075.0</v>
+        <v>3062.0</v>
       </c>
       <c r="E23" s="67">
         <f t="shared" si="2"/>
-        <v>0.6753678422</v>
+        <v>0.6949863291</v>
       </c>
       <c r="F23" s="76">
         <v>1.0</v>
@@ -2024,17 +2027,17 @@
       </c>
       <c r="B24" s="67">
         <f t="shared" si="1"/>
-        <v>0.01781245473</v>
+        <v>0.01835972393</v>
       </c>
       <c r="C24" s="69">
-        <v>400394.0</v>
+        <v>388459.0</v>
       </c>
       <c r="D24" s="69">
         <v>7132.0</v>
       </c>
       <c r="E24" s="67">
         <f t="shared" si="2"/>
-        <v>0.5787761143</v>
+        <v>0.5946030793</v>
       </c>
       <c r="F24" s="76">
         <v>1.0</v>
@@ -2046,17 +2049,17 @@
       </c>
       <c r="B25" s="67">
         <f t="shared" si="1"/>
-        <v>0.01723550958</v>
+        <v>0.01736281183</v>
       </c>
       <c r="C25" s="69">
-        <v>487598.0</v>
+        <v>473656.0</v>
       </c>
       <c r="D25" s="69">
-        <v>8404.0</v>
+        <v>8224.0</v>
       </c>
       <c r="E25" s="67">
         <f t="shared" si="2"/>
-        <v>0.4935661359</v>
+        <v>0.5061781259</v>
       </c>
       <c r="F25" s="76">
         <v>1.0</v>
@@ -2068,17 +2071,17 @@
       </c>
       <c r="B26" s="67">
         <f t="shared" si="1"/>
-        <v>0.007087833772</v>
+        <v>0.007348057912</v>
       </c>
       <c r="C26" s="69">
-        <v>437087.0</v>
+        <v>421608.0</v>
       </c>
       <c r="D26" s="69">
         <v>3098.0</v>
       </c>
       <c r="E26" s="67">
         <f t="shared" si="2"/>
-        <v>0.4353167614</v>
+        <v>0.4463227087</v>
       </c>
       <c r="F26" s="76">
         <v>1.0</v>
@@ -2090,17 +2093,17 @@
       </c>
       <c r="B27" s="67">
         <f t="shared" si="1"/>
-        <v>0.02438411649</v>
+        <v>0.0254128384</v>
       </c>
       <c r="C27" s="69">
-        <v>390090.0</v>
+        <v>374299.0</v>
       </c>
       <c r="D27" s="69">
         <v>9512.0</v>
       </c>
       <c r="E27" s="67">
         <f t="shared" si="2"/>
-        <v>0.395643149</v>
+        <v>0.405801008</v>
       </c>
       <c r="F27" s="76">
         <v>1.0</v>
@@ -2112,17 +2115,17 @@
       </c>
       <c r="B28" s="67">
         <f t="shared" si="1"/>
-        <v>0.01278968436</v>
+        <v>0.01331426098</v>
       </c>
       <c r="C28" s="69">
-        <v>276551.0</v>
+        <v>265655.0</v>
       </c>
       <c r="D28" s="69">
         <v>3537.0</v>
       </c>
       <c r="E28" s="67">
         <f t="shared" si="2"/>
-        <v>0.3711174189</v>
+        <v>0.3806984303</v>
       </c>
       <c r="F28" s="76">
         <v>1.0</v>
@@ -2134,17 +2137,17 @@
       </c>
       <c r="B29" s="71">
         <f t="shared" si="1"/>
-        <v>0.00596017411</v>
+        <v>0.005765633256</v>
       </c>
       <c r="C29" s="72">
-        <v>291770.0</v>
+        <v>280108.0</v>
       </c>
       <c r="D29" s="72">
-        <v>1739.0</v>
+        <v>1615.0</v>
       </c>
       <c r="E29" s="71">
         <f t="shared" si="2"/>
-        <v>0.348000394</v>
+        <v>0.3570113323</v>
       </c>
       <c r="F29" s="77">
         <v>1.0</v>
@@ -2749,18 +2752,18 @@
         <v>0.9</v>
       </c>
       <c r="C6" s="96">
-        <v>4608808.0</v>
+        <v>4433708.0</v>
       </c>
       <c r="D6" s="96">
-        <v>1603867.0</v>
+        <v>1582884.0</v>
       </c>
       <c r="E6" s="95">
         <f t="shared" ref="E6:E15" si="1">D6/C6</f>
-        <v>0.348000394</v>
+        <v>0.3570113323</v>
       </c>
       <c r="F6" s="95">
         <f>E6-B6</f>
-        <v>-0.551999606</v>
+        <v>-0.5429886677</v>
       </c>
     </row>
     <row r="7" ht="12.75" customHeight="1">
@@ -3027,18 +3030,18 @@
       </c>
       <c r="B6" s="95"/>
       <c r="C6" s="96">
-        <v>497114.0</v>
+        <v>325056.0</v>
       </c>
       <c r="D6" s="96">
-        <v>502.0</v>
+        <v>849.0</v>
       </c>
       <c r="E6" s="98">
         <f t="shared" ref="E6:E34" si="1">D6/C6</f>
-        <v>0.001009828731</v>
+        <v>0.002611857649</v>
       </c>
       <c r="F6" s="95">
         <f>E6-B6</f>
-        <v>0.001009828731</v>
+        <v>0.002611857649</v>
       </c>
     </row>
     <row r="7" ht="12.75" customHeight="1">
@@ -3047,16 +3050,18 @@
       </c>
       <c r="B7" s="95"/>
       <c r="C7" s="96">
-        <v>289943.0</v>
+        <v>497114.0</v>
       </c>
       <c r="D7" s="96">
-        <v>18524.0</v>
+        <v>502.0</v>
       </c>
       <c r="E7" s="98">
         <f t="shared" si="1"/>
-        <v>0.06388841945</v>
-      </c>
-      <c r="F7" s="95"/>
+        <v>0.001009828731</v>
+      </c>
+      <c r="F7" s="95" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="8" ht="12.75" customHeight="1">
       <c r="A8" s="94" t="s">
@@ -3064,14 +3069,14 @@
       </c>
       <c r="B8" s="95"/>
       <c r="C8" s="96">
-        <v>376294.0</v>
+        <v>347442.0</v>
       </c>
       <c r="D8" s="96">
-        <v>0.0</v>
+        <v>3420.0</v>
       </c>
       <c r="E8" s="98">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>0.009843369541</v>
       </c>
       <c r="F8" s="95"/>
     </row>
@@ -3081,7 +3086,7 @@
       </c>
       <c r="B9" s="95"/>
       <c r="C9" s="96">
-        <v>300241.0</v>
+        <v>376294.0</v>
       </c>
       <c r="D9" s="96">
         <v>0.0</v>
@@ -3098,14 +3103,14 @@
       </c>
       <c r="B10" s="95"/>
       <c r="C10" s="96">
-        <v>164240.0</v>
+        <v>300241.0</v>
       </c>
       <c r="D10" s="96">
-        <v>33288.0</v>
+        <v>0.0</v>
       </c>
       <c r="E10" s="98">
         <f t="shared" si="1"/>
-        <v>0.2026790063</v>
+        <v>0</v>
       </c>
       <c r="F10" s="95"/>
     </row>
@@ -3115,14 +3120,14 @@
       </c>
       <c r="B11" s="95"/>
       <c r="C11" s="96">
-        <v>325056.0</v>
+        <v>164240.0</v>
       </c>
       <c r="D11" s="96">
-        <v>849.0</v>
+        <v>33288.0</v>
       </c>
       <c r="E11" s="98">
         <f t="shared" si="1"/>
-        <v>0.002611857649</v>
+        <v>0.2026790063</v>
       </c>
       <c r="F11" s="95"/>
     </row>
@@ -3132,14 +3137,14 @@
       </c>
       <c r="B12" s="95"/>
       <c r="C12" s="96">
-        <v>280286.0</v>
+        <v>1367428.0</v>
       </c>
       <c r="D12" s="96">
-        <v>73.0</v>
+        <v>242701.0</v>
       </c>
       <c r="E12" s="98">
         <f t="shared" si="1"/>
-        <v>0.0002604482564</v>
+        <v>0.1774872242</v>
       </c>
       <c r="F12" s="95"/>
     </row>
@@ -3149,14 +3154,14 @@
       </c>
       <c r="B13" s="95"/>
       <c r="C13" s="96">
-        <v>96222.0</v>
+        <v>1365393.0</v>
       </c>
       <c r="D13" s="96">
-        <v>0.0</v>
+        <v>829916.0</v>
       </c>
       <c r="E13" s="98">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>0.6078220703</v>
       </c>
       <c r="F13" s="95"/>
     </row>
@@ -3166,7 +3171,7 @@
       </c>
       <c r="B14" s="95"/>
       <c r="C14" s="96">
-        <v>109883.0</v>
+        <v>96222.0</v>
       </c>
       <c r="D14" s="96">
         <v>0.0</v>
@@ -3183,14 +3188,14 @@
       </c>
       <c r="B15" s="95"/>
       <c r="C15" s="96">
-        <v>1365393.0</v>
+        <v>852822.0</v>
       </c>
       <c r="D15" s="96">
-        <v>829916.0</v>
+        <v>338231.0</v>
       </c>
       <c r="E15" s="98">
         <f t="shared" si="1"/>
-        <v>0.6078220703</v>
+        <v>0.3966021045</v>
       </c>
       <c r="F15" s="95"/>
     </row>
@@ -3200,14 +3205,14 @@
       </c>
       <c r="B16" s="95"/>
       <c r="C16" s="96">
-        <v>1367428.0</v>
+        <v>723363.0</v>
       </c>
       <c r="D16" s="96">
-        <v>242701.0</v>
+        <v>5147.0</v>
       </c>
       <c r="E16" s="98">
         <f t="shared" si="1"/>
-        <v>0.1774872242</v>
+        <v>0.007115376374</v>
       </c>
       <c r="F16" s="95"/>
     </row>
@@ -3217,14 +3222,14 @@
       </c>
       <c r="B17" s="95"/>
       <c r="C17" s="96">
-        <v>382369.0</v>
+        <v>109883.0</v>
       </c>
       <c r="D17" s="96">
-        <v>5900.0</v>
+        <v>0.0</v>
       </c>
       <c r="E17" s="98">
         <f t="shared" si="1"/>
-        <v>0.01543012117</v>
+        <v>0</v>
       </c>
       <c r="F17" s="95"/>
     </row>
@@ -3234,14 +3239,14 @@
       </c>
       <c r="B18" s="95"/>
       <c r="C18" s="96">
-        <v>379657.0</v>
+        <v>382369.0</v>
       </c>
       <c r="D18" s="96">
-        <v>0.0</v>
+        <v>5900.0</v>
       </c>
       <c r="E18" s="98">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>0.01543012117</v>
       </c>
       <c r="F18" s="95"/>
     </row>
@@ -3251,7 +3256,7 @@
       </c>
       <c r="B19" s="95"/>
       <c r="C19" s="96">
-        <v>263494.0</v>
+        <v>379657.0</v>
       </c>
       <c r="D19" s="96">
         <v>0.0</v>
@@ -3268,14 +3273,14 @@
       </c>
       <c r="B20" s="95"/>
       <c r="C20" s="96">
-        <v>723363.0</v>
+        <v>263494.0</v>
       </c>
       <c r="D20" s="96">
-        <v>5147.0</v>
+        <v>0.0</v>
       </c>
       <c r="E20" s="98">
         <f t="shared" si="1"/>
-        <v>0.007115376374</v>
+        <v>0</v>
       </c>
       <c r="F20" s="95"/>
     </row>
@@ -3285,14 +3290,14 @@
       </c>
       <c r="B21" s="95"/>
       <c r="C21" s="96">
-        <v>129383.0</v>
+        <v>328618.0</v>
       </c>
       <c r="D21" s="96">
-        <v>0.0</v>
+        <v>2607.0</v>
       </c>
       <c r="E21" s="98">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>0.007933223378</v>
       </c>
       <c r="F21" s="95"/>
     </row>
@@ -3302,7 +3307,7 @@
       </c>
       <c r="B22" s="95"/>
       <c r="C22" s="96">
-        <v>123280.0</v>
+        <v>129383.0</v>
       </c>
       <c r="D22" s="96">
         <v>0.0</v>
@@ -3319,7 +3324,7 @@
       </c>
       <c r="B23" s="95"/>
       <c r="C23" s="96">
-        <v>56621.0</v>
+        <v>200778.0</v>
       </c>
       <c r="D23" s="96">
         <v>0.0</v>
@@ -3353,14 +3358,14 @@
       </c>
       <c r="B25" s="95"/>
       <c r="C25" s="96">
-        <v>347442.0</v>
+        <v>832888.0</v>
       </c>
       <c r="D25" s="96">
-        <v>3420.0</v>
+        <v>10839.0</v>
       </c>
       <c r="E25" s="98">
         <f t="shared" si="1"/>
-        <v>0.009843369541</v>
+        <v>0.01301375455</v>
       </c>
       <c r="F25" s="95"/>
     </row>
@@ -3370,14 +3375,14 @@
       </c>
       <c r="B26" s="95"/>
       <c r="C26" s="96">
-        <v>365056.0</v>
+        <v>56621.0</v>
       </c>
       <c r="D26" s="96">
-        <v>1404.0</v>
+        <v>0.0</v>
       </c>
       <c r="E26" s="98">
         <f t="shared" si="1"/>
-        <v>0.003845985273</v>
+        <v>0</v>
       </c>
       <c r="F26" s="95"/>
     </row>
@@ -3404,14 +3409,14 @@
       </c>
       <c r="B28" s="95"/>
       <c r="C28" s="96">
-        <v>320082.0</v>
+        <v>280286.0</v>
       </c>
       <c r="D28" s="96">
-        <v>0.0</v>
+        <v>73.0</v>
       </c>
       <c r="E28" s="98">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>0.0002604482564</v>
       </c>
       <c r="F28" s="95"/>
     </row>
@@ -3421,7 +3426,7 @@
       </c>
       <c r="B29" s="95"/>
       <c r="C29" s="96">
-        <v>200778.0</v>
+        <v>123280.0</v>
       </c>
       <c r="D29" s="96">
         <v>0.0</v>
@@ -3438,14 +3443,14 @@
       </c>
       <c r="B30" s="95"/>
       <c r="C30" s="96">
-        <v>152565.0</v>
+        <v>365056.0</v>
       </c>
       <c r="D30" s="96">
-        <v>188.0</v>
+        <v>1404.0</v>
       </c>
       <c r="E30" s="98">
         <f t="shared" si="1"/>
-        <v>0.001232261659</v>
+        <v>0.003845985273</v>
       </c>
       <c r="F30" s="95"/>
     </row>
@@ -3455,14 +3460,14 @@
       </c>
       <c r="B31" s="95"/>
       <c r="C31" s="96">
-        <v>852822.0</v>
+        <v>320082.0</v>
       </c>
       <c r="D31" s="96">
-        <v>338231.0</v>
+        <v>0.0</v>
       </c>
       <c r="E31" s="98">
         <f t="shared" si="1"/>
-        <v>0.3966021045</v>
+        <v>0</v>
       </c>
       <c r="F31" s="95"/>
     </row>
@@ -3472,14 +3477,14 @@
       </c>
       <c r="B32" s="95"/>
       <c r="C32" s="96">
-        <v>328618.0</v>
+        <v>289943.0</v>
       </c>
       <c r="D32" s="96">
-        <v>2607.0</v>
+        <v>18524.0</v>
       </c>
       <c r="E32" s="98">
         <f t="shared" si="1"/>
-        <v>0.007933223378</v>
+        <v>0.06388841945</v>
       </c>
       <c r="F32" s="95"/>
     </row>
@@ -3506,14 +3511,14 @@
       </c>
       <c r="B34" s="95"/>
       <c r="C34" s="96">
-        <v>1004515.0</v>
+        <v>152565.0</v>
       </c>
       <c r="D34" s="96">
-        <v>20983.0</v>
+        <v>188.0</v>
       </c>
       <c r="E34" s="98">
         <f t="shared" si="1"/>
-        <v>0.02088868758</v>
+        <v>0.001232261659</v>
       </c>
       <c r="F34" s="95"/>
     </row>
@@ -3581,16 +3586,24 @@
       </c>
     </row>
     <row r="4" ht="15.75" customHeight="1">
-      <c r="A4" s="103"/>
-      <c r="B4" s="101"/>
-      <c r="C4" s="104"/>
-      <c r="D4" s="101"/>
+      <c r="A4" s="100">
+        <v>44351.0</v>
+      </c>
+      <c r="B4" s="101" t="s">
+        <v>159</v>
+      </c>
+      <c r="C4" s="103">
+        <v>2020.0</v>
+      </c>
+      <c r="D4" s="101" t="s">
+        <v>160</v>
+      </c>
     </row>
     <row r="5" ht="15.75" customHeight="1">
       <c r="A5" s="100"/>
-      <c r="B5" s="105"/>
-      <c r="C5" s="106"/>
-      <c r="D5" s="107"/>
+      <c r="B5" s="104"/>
+      <c r="C5" s="105"/>
+      <c r="D5" s="106"/>
     </row>
   </sheetData>
   <drawing r:id="rId1"/>

</xml_diff>

<commit_message>
202106 release uk (#41)
* UK removed in RP3

* download files updated

* Updates June release with May data
</commit_message>
<xml_diff>
--- a/static/download/2020/RP3_ERT_ATFM_2020_Jan_Dec.xlsx
+++ b/static/download/2020/RP3_ERT_ATFM_2020_Jan_Dec.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="215" uniqueCount="159">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="218" uniqueCount="161">
   <si>
     <t>Data source</t>
   </si>
@@ -47,7 +47,7 @@
     <t>Period: JAN-DEC</t>
   </si>
   <si>
-    <t>SES Area</t>
+    <t>SES Area (RP3)</t>
   </si>
   <si>
     <t>Area</t>
@@ -74,7 +74,7 @@
     <t>% of flights with en-route ATFM delay greater than 15 min</t>
   </si>
   <si>
-    <t>SES area</t>
+    <t>SES area (RP3)</t>
   </si>
   <si>
     <t xml:space="preserve">2015 </t>
@@ -389,93 +389,93 @@
     <t>Entity</t>
   </si>
   <si>
+    <t>ANS CR</t>
+  </si>
+  <si>
     <t>Austro Control</t>
   </si>
   <si>
+    <t>Avinor</t>
+  </si>
+  <si>
+    <t>BULATSA</t>
+  </si>
+  <si>
+    <t>Croatia Control</t>
+  </si>
+  <si>
+    <t>DCAC Cyprus</t>
+  </si>
+  <si>
+    <t>DFS</t>
+  </si>
+  <si>
+    <t>DSNA</t>
+  </si>
+  <si>
+    <t>EANS</t>
+  </si>
+  <si>
+    <t>ENAIRE</t>
+  </si>
+  <si>
+    <t>ENAV</t>
+  </si>
+  <si>
+    <t>Fintraffic ANS</t>
+  </si>
+  <si>
+    <t>HCAA</t>
+  </si>
+  <si>
+    <t>HungaroControl (EC)</t>
+  </si>
+  <si>
+    <t>IAA</t>
+  </si>
+  <si>
+    <t>LFV</t>
+  </si>
+  <si>
+    <t>LGS</t>
+  </si>
+  <si>
+    <t>LPS</t>
+  </si>
+  <si>
+    <t>LVNL</t>
+  </si>
+  <si>
+    <t>Maastricht UAC</t>
+  </si>
+  <si>
+    <t>MATS</t>
+  </si>
+  <si>
+    <t>NAV Portugal</t>
+  </si>
+  <si>
+    <t>NAVIAIR</t>
+  </si>
+  <si>
+    <t>Oro navigacija</t>
+  </si>
+  <si>
+    <t>PANSA</t>
+  </si>
+  <si>
+    <t>ROMATSA</t>
+  </si>
+  <si>
     <t>skeyes</t>
   </si>
   <si>
-    <t>BULATSA</t>
-  </si>
-  <si>
-    <t>Croatia Control</t>
-  </si>
-  <si>
-    <t>DCAC Cyprus</t>
-  </si>
-  <si>
-    <t>ANS CR</t>
-  </si>
-  <si>
-    <t>NAVIAIR</t>
-  </si>
-  <si>
-    <t>EANS</t>
-  </si>
-  <si>
-    <t>Fintraffic ANS</t>
-  </si>
-  <si>
-    <t>DSNA</t>
-  </si>
-  <si>
-    <t>DFS</t>
-  </si>
-  <si>
-    <t>HCAA</t>
-  </si>
-  <si>
-    <t>HungaroControl (EC)</t>
-  </si>
-  <si>
-    <t>IAA</t>
-  </si>
-  <si>
-    <t>ENAV</t>
-  </si>
-  <si>
-    <t>LGS</t>
-  </si>
-  <si>
-    <t>Oro navigacija</t>
-  </si>
-  <si>
-    <t>MATS</t>
-  </si>
-  <si>
-    <t>LVNL</t>
-  </si>
-  <si>
-    <t>Avinor</t>
-  </si>
-  <si>
-    <t>PANSA</t>
-  </si>
-  <si>
-    <t>NAV Portugal</t>
-  </si>
-  <si>
-    <t>ROMATSA</t>
-  </si>
-  <si>
-    <t>LPS</t>
+    <t>Skyguide</t>
   </si>
   <si>
     <t>Slovenia Control</t>
   </si>
   <si>
-    <t>ENAIRE</t>
-  </si>
-  <si>
-    <t>LFV</t>
-  </si>
-  <si>
-    <t>Skyguide</t>
-  </si>
-  <si>
-    <t>NATS (Continental)</t>
-  </si>
-  <si>
     <t>Change date</t>
   </si>
   <si>
@@ -492,6 +492,12 @@
   </si>
   <si>
     <t>Local level changed to ANSP</t>
+  </si>
+  <si>
+    <t>UK</t>
+  </si>
+  <si>
+    <t>UK removed</t>
   </si>
 </sst>
 </file>
@@ -847,7 +853,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="108">
+  <cellXfs count="107">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -1152,9 +1158,6 @@
     </xf>
     <xf borderId="0" fillId="3" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="0" fillId="3" fontId="10" numFmtId="164" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
-      <alignment horizontal="center" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="10" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0" shrinkToFit="0" wrapText="0"/>
@@ -1244,7 +1247,7 @@
         <v>4</v>
       </c>
       <c r="B2" s="10">
-        <v>44308.0</v>
+        <v>44351.0</v>
       </c>
       <c r="C2" s="11" t="s">
         <v>5</v>
@@ -1330,21 +1333,21 @@
       </c>
       <c r="C6" s="31">
         <f t="shared" ref="C6:C11" si="1">E6/D6</f>
-        <v>0.7608276904</v>
+        <v>0.7757046325</v>
       </c>
       <c r="D6" s="32">
-        <v>9242345.0</v>
+        <v>8820414.0</v>
       </c>
       <c r="E6" s="33">
-        <v>7031832.0</v>
+        <v>6842036.0</v>
       </c>
       <c r="F6" s="34"/>
       <c r="G6" s="35">
         <f t="shared" ref="G6:G11" si="2">C6-F6</f>
-        <v>0.7608276904</v>
+        <v>0.7757046325</v>
       </c>
       <c r="H6" s="36">
-        <v>0.019</v>
+        <v>0.0193</v>
       </c>
     </row>
     <row r="7" ht="12.0" customHeight="1">
@@ -1356,21 +1359,21 @@
       </c>
       <c r="C7" s="31">
         <f t="shared" si="1"/>
-        <v>0.9143127931</v>
+        <v>0.8742416857</v>
       </c>
       <c r="D7" s="38">
-        <v>9505573.0</v>
+        <v>9086437.0</v>
       </c>
       <c r="E7" s="39">
-        <v>8691067.0</v>
+        <v>7943742.0</v>
       </c>
       <c r="F7" s="40"/>
       <c r="G7" s="41">
         <f t="shared" si="2"/>
-        <v>0.9143127931</v>
+        <v>0.8742416857</v>
       </c>
       <c r="H7" s="36">
-        <v>0.0217</v>
+        <v>0.0206</v>
       </c>
     </row>
     <row r="8" ht="12.0" customHeight="1">
@@ -1382,21 +1385,21 @@
       </c>
       <c r="C8" s="31">
         <f t="shared" si="1"/>
-        <v>0.941046466</v>
+        <v>0.938859843</v>
       </c>
       <c r="D8" s="38">
-        <v>9847620.0</v>
+        <v>9425491.0</v>
       </c>
       <c r="E8" s="39">
-        <v>9267068.0</v>
+        <v>8849215.0</v>
       </c>
       <c r="F8" s="34"/>
       <c r="G8" s="41">
         <f t="shared" si="2"/>
-        <v>0.941046466</v>
+        <v>0.938859843</v>
       </c>
       <c r="H8" s="36">
-        <v>0.0218</v>
+        <v>0.0217</v>
       </c>
     </row>
     <row r="9" ht="12.0" customHeight="1">
@@ -1408,21 +1411,21 @@
       </c>
       <c r="C9" s="31">
         <f t="shared" si="1"/>
-        <v>1.827205784</v>
+        <v>1.830159819</v>
       </c>
       <c r="D9" s="38">
-        <v>1.0215122E7</v>
+        <v>9800596.0</v>
       </c>
       <c r="E9" s="39">
-        <v>1.866513E7</v>
+        <v>1.7936657E7</v>
       </c>
       <c r="F9" s="34"/>
       <c r="G9" s="41">
         <f t="shared" si="2"/>
-        <v>1.827205784</v>
+        <v>1.830159819</v>
       </c>
       <c r="H9" s="36">
-        <v>0.0437</v>
+        <v>0.0438</v>
       </c>
     </row>
     <row r="10" ht="12.0" customHeight="1">
@@ -1434,21 +1437,21 @@
       </c>
       <c r="C10" s="31">
         <f t="shared" si="1"/>
-        <v>1.666567384</v>
+        <v>1.679992502</v>
       </c>
       <c r="D10" s="38">
-        <v>1.0334109E7</v>
+        <v>9933936.0</v>
       </c>
       <c r="E10" s="39">
-        <v>1.7222489E7</v>
+        <v>1.6688938E7</v>
       </c>
       <c r="F10" s="34"/>
       <c r="G10" s="41">
         <f t="shared" si="2"/>
-        <v>1.666567384</v>
+        <v>1.679992502</v>
       </c>
       <c r="H10" s="36">
-        <v>0.0391</v>
+        <v>0.0394</v>
       </c>
     </row>
     <row r="11" ht="12.0" customHeight="1">
@@ -1460,23 +1463,23 @@
       </c>
       <c r="C11" s="31">
         <f t="shared" si="1"/>
-        <v>0.348000394</v>
+        <v>0.3570113323</v>
       </c>
       <c r="D11" s="38">
-        <v>4608808.0</v>
+        <v>4433708.0</v>
       </c>
       <c r="E11" s="39">
-        <v>1603867.0</v>
+        <v>1582884.0</v>
       </c>
       <c r="F11" s="42">
         <v>0.9</v>
       </c>
       <c r="G11" s="41">
         <f t="shared" si="2"/>
-        <v>-0.551999606</v>
+        <v>-0.5429886677</v>
       </c>
       <c r="H11" s="36">
-        <v>0.0071</v>
+        <v>0.0072</v>
       </c>
     </row>
     <row r="12" ht="12.0" customHeight="1">
@@ -1597,7 +1600,7 @@
         <v>4</v>
       </c>
       <c r="B2" s="10">
-        <v>44308.0</v>
+        <v>44351.0</v>
       </c>
       <c r="C2" s="11" t="s">
         <v>5</v>
@@ -1662,13 +1665,13 @@
       </c>
       <c r="B6" s="62">
         <f t="shared" ref="B6:B29" si="1">D6/C6</f>
-        <v>0.3881771646</v>
+        <v>0.4041344334</v>
       </c>
       <c r="C6" s="63">
-        <v>730620.0</v>
+        <v>699975.0</v>
       </c>
       <c r="D6" s="64">
-        <v>283610.0</v>
+        <v>282884.0</v>
       </c>
       <c r="E6" s="65"/>
       <c r="F6" s="66">
@@ -1681,13 +1684,13 @@
       </c>
       <c r="B7" s="67">
         <f t="shared" si="1"/>
-        <v>0.4865745041</v>
+        <v>0.4933644225</v>
       </c>
       <c r="C7" s="68">
-        <v>686902.0</v>
+        <v>657893.0</v>
       </c>
       <c r="D7" s="69">
-        <v>334229.0</v>
+        <v>324581.0</v>
       </c>
       <c r="E7" s="65"/>
       <c r="F7" s="66">
@@ -1700,13 +1703,13 @@
       </c>
       <c r="B8" s="67">
         <f t="shared" si="1"/>
-        <v>0.9718605532</v>
+        <v>1.012783337</v>
       </c>
       <c r="C8" s="68">
-        <v>786938.0</v>
+        <v>753872.0</v>
       </c>
       <c r="D8" s="69">
-        <v>764794.0</v>
+        <v>763509.0</v>
       </c>
       <c r="E8" s="65"/>
       <c r="F8" s="66">
@@ -1719,13 +1722,13 @@
       </c>
       <c r="B9" s="67">
         <f t="shared" si="1"/>
-        <v>1.133095043</v>
+        <v>1.148831511</v>
       </c>
       <c r="C9" s="69">
-        <v>848544.0</v>
+        <v>815412.0</v>
       </c>
       <c r="D9" s="69">
-        <v>961481.0</v>
+        <v>936771.0</v>
       </c>
       <c r="E9" s="65"/>
       <c r="F9" s="66">
@@ -1738,13 +1741,13 @@
       </c>
       <c r="B10" s="67">
         <f t="shared" si="1"/>
-        <v>1.858407406</v>
+        <v>1.914318462</v>
       </c>
       <c r="C10" s="69">
-        <v>921729.0</v>
+        <v>886422.0</v>
       </c>
       <c r="D10" s="69">
-        <v>1712948.0</v>
+        <v>1696894.0</v>
       </c>
       <c r="E10" s="65"/>
       <c r="F10" s="66">
@@ -1757,13 +1760,13 @@
       </c>
       <c r="B11" s="67">
         <f t="shared" si="1"/>
-        <v>2.957661543</v>
+        <v>2.988936024</v>
       </c>
       <c r="C11" s="69">
-        <v>966757.0</v>
+        <v>932305.0</v>
       </c>
       <c r="D11" s="69">
-        <v>2859340.0</v>
+        <v>2786600.0</v>
       </c>
       <c r="E11" s="65"/>
       <c r="F11" s="66">
@@ -1776,13 +1779,13 @@
       </c>
       <c r="B12" s="67">
         <f t="shared" si="1"/>
-        <v>3.379891483</v>
+        <v>3.369078543</v>
       </c>
       <c r="C12" s="69">
-        <v>1018454.0</v>
+        <v>982444.0</v>
       </c>
       <c r="D12" s="69">
-        <v>3442264.0</v>
+        <v>3309931.0</v>
       </c>
       <c r="E12" s="70" t="s">
         <v>8</v>
@@ -1797,13 +1800,13 @@
       </c>
       <c r="B13" s="67">
         <f t="shared" si="1"/>
-        <v>2.844248328</v>
+        <v>2.808366039</v>
       </c>
       <c r="C13" s="69">
-        <v>1005864.0</v>
+        <v>970256.0</v>
       </c>
       <c r="D13" s="69">
-        <v>2860927.0</v>
+        <v>2724834.0</v>
       </c>
       <c r="E13" s="65"/>
       <c r="F13" s="66">
@@ -1816,13 +1819,13 @@
       </c>
       <c r="B14" s="67">
         <f t="shared" si="1"/>
-        <v>1.905906347</v>
+        <v>1.895806678</v>
       </c>
       <c r="C14" s="69">
-        <v>966909.0</v>
+        <v>932411.0</v>
       </c>
       <c r="D14" s="69">
-        <v>1842838.0</v>
+        <v>1767671.0</v>
       </c>
       <c r="E14" s="65"/>
       <c r="F14" s="66">
@@ -1835,13 +1838,13 @@
       </c>
       <c r="B15" s="67">
         <f t="shared" si="1"/>
-        <v>1.063593354</v>
+        <v>1.049598995</v>
       </c>
       <c r="C15" s="69">
-        <v>915646.0</v>
+        <v>880038.0</v>
       </c>
       <c r="D15" s="69">
-        <v>973875.0</v>
+        <v>923687.0</v>
       </c>
       <c r="E15" s="65"/>
       <c r="F15" s="66">
@@ -1854,13 +1857,13 @@
       </c>
       <c r="B16" s="67">
         <f t="shared" si="1"/>
-        <v>0.3414012739</v>
+        <v>0.3515899995</v>
       </c>
       <c r="C16" s="69">
-        <v>745750.0</v>
+        <v>713365.0</v>
       </c>
       <c r="D16" s="69">
-        <v>254600.0</v>
+        <v>250812.0</v>
       </c>
       <c r="E16" s="65"/>
       <c r="F16" s="66">
@@ -1873,13 +1876,13 @@
       </c>
       <c r="B17" s="71">
         <f t="shared" si="1"/>
-        <v>1.258902751</v>
+        <v>1.297685975</v>
       </c>
       <c r="C17" s="72">
-        <v>739996.0</v>
+        <v>709543.0</v>
       </c>
       <c r="D17" s="72">
-        <v>931583.0</v>
+        <v>920764.0</v>
       </c>
       <c r="E17" s="73"/>
       <c r="F17" s="66">
@@ -1892,17 +1895,17 @@
       </c>
       <c r="B18" s="62">
         <f t="shared" si="1"/>
-        <v>0.5024975326</v>
+        <v>0.5179546649</v>
       </c>
       <c r="C18" s="64">
-        <v>729520.0</v>
+        <v>700208.0</v>
       </c>
       <c r="D18" s="64">
-        <v>366582.0</v>
+        <v>362676.0</v>
       </c>
       <c r="E18" s="74">
         <f>D18/C18</f>
-        <v>0.5024975326</v>
+        <v>0.5179546649</v>
       </c>
       <c r="F18" s="75">
         <v>1.0</v>
@@ -1914,17 +1917,17 @@
       </c>
       <c r="B19" s="67">
         <f t="shared" si="1"/>
-        <v>0.8431746872</v>
+        <v>0.8578355891</v>
       </c>
       <c r="C19" s="69">
-        <v>695111.0</v>
+        <v>666306.0</v>
       </c>
       <c r="D19" s="69">
-        <v>586100.0</v>
+        <v>571581.0</v>
       </c>
       <c r="E19" s="67">
         <f t="shared" ref="E19:E29" si="2">sum(D$18:D19)/sum(C$18:C19)</f>
-        <v>0.6687219357</v>
+        <v>0.6836790549</v>
       </c>
       <c r="F19" s="76">
         <v>1.0</v>
@@ -1936,17 +1939,17 @@
       </c>
       <c r="B20" s="67">
         <f t="shared" si="1"/>
-        <v>1.318724928</v>
+        <v>1.374425536</v>
       </c>
       <c r="C20" s="69">
-        <v>463660.0</v>
+        <v>443239.0</v>
       </c>
       <c r="D20" s="69">
-        <v>611440.0</v>
+        <v>609199.0</v>
       </c>
       <c r="E20" s="67">
         <f t="shared" si="2"/>
-        <v>0.828326778</v>
+        <v>0.8528545056</v>
       </c>
       <c r="F20" s="76">
         <v>1.0</v>
@@ -1958,17 +1961,17 @@
       </c>
       <c r="B21" s="67">
         <f t="shared" si="1"/>
-        <v>0.001483809025</v>
+        <v>0.001553583396</v>
       </c>
       <c r="C21" s="69">
-        <v>103113.0</v>
+        <v>98482.0</v>
       </c>
       <c r="D21" s="69">
         <v>153.0</v>
       </c>
       <c r="E21" s="67">
         <f t="shared" si="2"/>
-        <v>0.7855136376</v>
+        <v>0.8089197609</v>
       </c>
       <c r="F21" s="76">
         <v>1.0</v>
@@ -1980,17 +1983,17 @@
       </c>
       <c r="B22" s="67">
         <f t="shared" si="1"/>
-        <v>0.02324166829</v>
+        <v>0.02419386359</v>
       </c>
       <c r="C22" s="69">
-        <v>133166.0</v>
+        <v>127925.0</v>
       </c>
       <c r="D22" s="69">
         <v>3095.0</v>
       </c>
       <c r="E22" s="67">
         <f t="shared" si="2"/>
-        <v>0.7377351652</v>
+        <v>0.7596181047</v>
       </c>
       <c r="F22" s="76">
         <v>1.0</v>
@@ -2002,17 +2005,17 @@
       </c>
       <c r="B23" s="67">
         <f t="shared" si="1"/>
-        <v>0.01531771176</v>
+        <v>0.01580281065</v>
       </c>
       <c r="C23" s="69">
-        <v>200748.0</v>
+        <v>193763.0</v>
       </c>
       <c r="D23" s="69">
-        <v>3075.0</v>
+        <v>3062.0</v>
       </c>
       <c r="E23" s="67">
         <f t="shared" si="2"/>
-        <v>0.6753678422</v>
+        <v>0.6949863291</v>
       </c>
       <c r="F23" s="76">
         <v>1.0</v>
@@ -2024,17 +2027,17 @@
       </c>
       <c r="B24" s="67">
         <f t="shared" si="1"/>
-        <v>0.01781245473</v>
+        <v>0.01835972393</v>
       </c>
       <c r="C24" s="69">
-        <v>400394.0</v>
+        <v>388459.0</v>
       </c>
       <c r="D24" s="69">
         <v>7132.0</v>
       </c>
       <c r="E24" s="67">
         <f t="shared" si="2"/>
-        <v>0.5787761143</v>
+        <v>0.5946030793</v>
       </c>
       <c r="F24" s="76">
         <v>1.0</v>
@@ -2046,17 +2049,17 @@
       </c>
       <c r="B25" s="67">
         <f t="shared" si="1"/>
-        <v>0.01723550958</v>
+        <v>0.01736281183</v>
       </c>
       <c r="C25" s="69">
-        <v>487598.0</v>
+        <v>473656.0</v>
       </c>
       <c r="D25" s="69">
-        <v>8404.0</v>
+        <v>8224.0</v>
       </c>
       <c r="E25" s="67">
         <f t="shared" si="2"/>
-        <v>0.4935661359</v>
+        <v>0.5061781259</v>
       </c>
       <c r="F25" s="76">
         <v>1.0</v>
@@ -2068,17 +2071,17 @@
       </c>
       <c r="B26" s="67">
         <f t="shared" si="1"/>
-        <v>0.007087833772</v>
+        <v>0.007348057912</v>
       </c>
       <c r="C26" s="69">
-        <v>437087.0</v>
+        <v>421608.0</v>
       </c>
       <c r="D26" s="69">
         <v>3098.0</v>
       </c>
       <c r="E26" s="67">
         <f t="shared" si="2"/>
-        <v>0.4353167614</v>
+        <v>0.4463227087</v>
       </c>
       <c r="F26" s="76">
         <v>1.0</v>
@@ -2090,17 +2093,17 @@
       </c>
       <c r="B27" s="67">
         <f t="shared" si="1"/>
-        <v>0.02438411649</v>
+        <v>0.0254128384</v>
       </c>
       <c r="C27" s="69">
-        <v>390090.0</v>
+        <v>374299.0</v>
       </c>
       <c r="D27" s="69">
         <v>9512.0</v>
       </c>
       <c r="E27" s="67">
         <f t="shared" si="2"/>
-        <v>0.395643149</v>
+        <v>0.405801008</v>
       </c>
       <c r="F27" s="76">
         <v>1.0</v>
@@ -2112,17 +2115,17 @@
       </c>
       <c r="B28" s="67">
         <f t="shared" si="1"/>
-        <v>0.01278968436</v>
+        <v>0.01331426098</v>
       </c>
       <c r="C28" s="69">
-        <v>276551.0</v>
+        <v>265655.0</v>
       </c>
       <c r="D28" s="69">
         <v>3537.0</v>
       </c>
       <c r="E28" s="67">
         <f t="shared" si="2"/>
-        <v>0.3711174189</v>
+        <v>0.3806984303</v>
       </c>
       <c r="F28" s="76">
         <v>1.0</v>
@@ -2134,17 +2137,17 @@
       </c>
       <c r="B29" s="71">
         <f t="shared" si="1"/>
-        <v>0.00596017411</v>
+        <v>0.005765633256</v>
       </c>
       <c r="C29" s="72">
-        <v>291770.0</v>
+        <v>280108.0</v>
       </c>
       <c r="D29" s="72">
-        <v>1739.0</v>
+        <v>1615.0</v>
       </c>
       <c r="E29" s="71">
         <f t="shared" si="2"/>
-        <v>0.348000394</v>
+        <v>0.3570113323</v>
       </c>
       <c r="F29" s="77">
         <v>1.0</v>
@@ -2749,18 +2752,18 @@
         <v>0.9</v>
       </c>
       <c r="C6" s="96">
-        <v>4608808.0</v>
+        <v>4433708.0</v>
       </c>
       <c r="D6" s="96">
-        <v>1603867.0</v>
+        <v>1582884.0</v>
       </c>
       <c r="E6" s="95">
         <f t="shared" ref="E6:E15" si="1">D6/C6</f>
-        <v>0.348000394</v>
+        <v>0.3570113323</v>
       </c>
       <c r="F6" s="95">
         <f>E6-B6</f>
-        <v>-0.551999606</v>
+        <v>-0.5429886677</v>
       </c>
     </row>
     <row r="7" ht="12.75" customHeight="1">
@@ -3027,18 +3030,18 @@
       </c>
       <c r="B6" s="95"/>
       <c r="C6" s="96">
-        <v>497114.0</v>
+        <v>325056.0</v>
       </c>
       <c r="D6" s="96">
-        <v>502.0</v>
+        <v>849.0</v>
       </c>
       <c r="E6" s="98">
         <f t="shared" ref="E6:E34" si="1">D6/C6</f>
-        <v>0.001009828731</v>
+        <v>0.002611857649</v>
       </c>
       <c r="F6" s="95">
         <f>E6-B6</f>
-        <v>0.001009828731</v>
+        <v>0.002611857649</v>
       </c>
     </row>
     <row r="7" ht="12.75" customHeight="1">
@@ -3047,16 +3050,18 @@
       </c>
       <c r="B7" s="95"/>
       <c r="C7" s="96">
-        <v>289943.0</v>
+        <v>497114.0</v>
       </c>
       <c r="D7" s="96">
-        <v>18524.0</v>
+        <v>502.0</v>
       </c>
       <c r="E7" s="98">
         <f t="shared" si="1"/>
-        <v>0.06388841945</v>
-      </c>
-      <c r="F7" s="95"/>
+        <v>0.001009828731</v>
+      </c>
+      <c r="F7" s="95" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="8" ht="12.75" customHeight="1">
       <c r="A8" s="94" t="s">
@@ -3064,14 +3069,14 @@
       </c>
       <c r="B8" s="95"/>
       <c r="C8" s="96">
-        <v>376294.0</v>
+        <v>347442.0</v>
       </c>
       <c r="D8" s="96">
-        <v>0.0</v>
+        <v>3420.0</v>
       </c>
       <c r="E8" s="98">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>0.009843369541</v>
       </c>
       <c r="F8" s="95"/>
     </row>
@@ -3081,7 +3086,7 @@
       </c>
       <c r="B9" s="95"/>
       <c r="C9" s="96">
-        <v>300241.0</v>
+        <v>376294.0</v>
       </c>
       <c r="D9" s="96">
         <v>0.0</v>
@@ -3098,14 +3103,14 @@
       </c>
       <c r="B10" s="95"/>
       <c r="C10" s="96">
-        <v>164240.0</v>
+        <v>300241.0</v>
       </c>
       <c r="D10" s="96">
-        <v>33288.0</v>
+        <v>0.0</v>
       </c>
       <c r="E10" s="98">
         <f t="shared" si="1"/>
-        <v>0.2026790063</v>
+        <v>0</v>
       </c>
       <c r="F10" s="95"/>
     </row>
@@ -3115,14 +3120,14 @@
       </c>
       <c r="B11" s="95"/>
       <c r="C11" s="96">
-        <v>325056.0</v>
+        <v>164240.0</v>
       </c>
       <c r="D11" s="96">
-        <v>849.0</v>
+        <v>33288.0</v>
       </c>
       <c r="E11" s="98">
         <f t="shared" si="1"/>
-        <v>0.002611857649</v>
+        <v>0.2026790063</v>
       </c>
       <c r="F11" s="95"/>
     </row>
@@ -3132,14 +3137,14 @@
       </c>
       <c r="B12" s="95"/>
       <c r="C12" s="96">
-        <v>280286.0</v>
+        <v>1367428.0</v>
       </c>
       <c r="D12" s="96">
-        <v>73.0</v>
+        <v>242701.0</v>
       </c>
       <c r="E12" s="98">
         <f t="shared" si="1"/>
-        <v>0.0002604482564</v>
+        <v>0.1774872242</v>
       </c>
       <c r="F12" s="95"/>
     </row>
@@ -3149,14 +3154,14 @@
       </c>
       <c r="B13" s="95"/>
       <c r="C13" s="96">
-        <v>96222.0</v>
+        <v>1365393.0</v>
       </c>
       <c r="D13" s="96">
-        <v>0.0</v>
+        <v>829916.0</v>
       </c>
       <c r="E13" s="98">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>0.6078220703</v>
       </c>
       <c r="F13" s="95"/>
     </row>
@@ -3166,7 +3171,7 @@
       </c>
       <c r="B14" s="95"/>
       <c r="C14" s="96">
-        <v>109883.0</v>
+        <v>96222.0</v>
       </c>
       <c r="D14" s="96">
         <v>0.0</v>
@@ -3183,14 +3188,14 @@
       </c>
       <c r="B15" s="95"/>
       <c r="C15" s="96">
-        <v>1365393.0</v>
+        <v>852822.0</v>
       </c>
       <c r="D15" s="96">
-        <v>829916.0</v>
+        <v>338231.0</v>
       </c>
       <c r="E15" s="98">
         <f t="shared" si="1"/>
-        <v>0.6078220703</v>
+        <v>0.3966021045</v>
       </c>
       <c r="F15" s="95"/>
     </row>
@@ -3200,14 +3205,14 @@
       </c>
       <c r="B16" s="95"/>
       <c r="C16" s="96">
-        <v>1367428.0</v>
+        <v>723363.0</v>
       </c>
       <c r="D16" s="96">
-        <v>242701.0</v>
+        <v>5147.0</v>
       </c>
       <c r="E16" s="98">
         <f t="shared" si="1"/>
-        <v>0.1774872242</v>
+        <v>0.007115376374</v>
       </c>
       <c r="F16" s="95"/>
     </row>
@@ -3217,14 +3222,14 @@
       </c>
       <c r="B17" s="95"/>
       <c r="C17" s="96">
-        <v>382369.0</v>
+        <v>109883.0</v>
       </c>
       <c r="D17" s="96">
-        <v>5900.0</v>
+        <v>0.0</v>
       </c>
       <c r="E17" s="98">
         <f t="shared" si="1"/>
-        <v>0.01543012117</v>
+        <v>0</v>
       </c>
       <c r="F17" s="95"/>
     </row>
@@ -3234,14 +3239,14 @@
       </c>
       <c r="B18" s="95"/>
       <c r="C18" s="96">
-        <v>379657.0</v>
+        <v>382369.0</v>
       </c>
       <c r="D18" s="96">
-        <v>0.0</v>
+        <v>5900.0</v>
       </c>
       <c r="E18" s="98">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>0.01543012117</v>
       </c>
       <c r="F18" s="95"/>
     </row>
@@ -3251,7 +3256,7 @@
       </c>
       <c r="B19" s="95"/>
       <c r="C19" s="96">
-        <v>263494.0</v>
+        <v>379657.0</v>
       </c>
       <c r="D19" s="96">
         <v>0.0</v>
@@ -3268,14 +3273,14 @@
       </c>
       <c r="B20" s="95"/>
       <c r="C20" s="96">
-        <v>723363.0</v>
+        <v>263494.0</v>
       </c>
       <c r="D20" s="96">
-        <v>5147.0</v>
+        <v>0.0</v>
       </c>
       <c r="E20" s="98">
         <f t="shared" si="1"/>
-        <v>0.007115376374</v>
+        <v>0</v>
       </c>
       <c r="F20" s="95"/>
     </row>
@@ -3285,14 +3290,14 @@
       </c>
       <c r="B21" s="95"/>
       <c r="C21" s="96">
-        <v>129383.0</v>
+        <v>328618.0</v>
       </c>
       <c r="D21" s="96">
-        <v>0.0</v>
+        <v>2607.0</v>
       </c>
       <c r="E21" s="98">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>0.007933223378</v>
       </c>
       <c r="F21" s="95"/>
     </row>
@@ -3302,7 +3307,7 @@
       </c>
       <c r="B22" s="95"/>
       <c r="C22" s="96">
-        <v>123280.0</v>
+        <v>129383.0</v>
       </c>
       <c r="D22" s="96">
         <v>0.0</v>
@@ -3319,7 +3324,7 @@
       </c>
       <c r="B23" s="95"/>
       <c r="C23" s="96">
-        <v>56621.0</v>
+        <v>200778.0</v>
       </c>
       <c r="D23" s="96">
         <v>0.0</v>
@@ -3353,14 +3358,14 @@
       </c>
       <c r="B25" s="95"/>
       <c r="C25" s="96">
-        <v>347442.0</v>
+        <v>832888.0</v>
       </c>
       <c r="D25" s="96">
-        <v>3420.0</v>
+        <v>10839.0</v>
       </c>
       <c r="E25" s="98">
         <f t="shared" si="1"/>
-        <v>0.009843369541</v>
+        <v>0.01301375455</v>
       </c>
       <c r="F25" s="95"/>
     </row>
@@ -3370,14 +3375,14 @@
       </c>
       <c r="B26" s="95"/>
       <c r="C26" s="96">
-        <v>365056.0</v>
+        <v>56621.0</v>
       </c>
       <c r="D26" s="96">
-        <v>1404.0</v>
+        <v>0.0</v>
       </c>
       <c r="E26" s="98">
         <f t="shared" si="1"/>
-        <v>0.003845985273</v>
+        <v>0</v>
       </c>
       <c r="F26" s="95"/>
     </row>
@@ -3404,14 +3409,14 @@
       </c>
       <c r="B28" s="95"/>
       <c r="C28" s="96">
-        <v>320082.0</v>
+        <v>280286.0</v>
       </c>
       <c r="D28" s="96">
-        <v>0.0</v>
+        <v>73.0</v>
       </c>
       <c r="E28" s="98">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>0.0002604482564</v>
       </c>
       <c r="F28" s="95"/>
     </row>
@@ -3421,7 +3426,7 @@
       </c>
       <c r="B29" s="95"/>
       <c r="C29" s="96">
-        <v>200778.0</v>
+        <v>123280.0</v>
       </c>
       <c r="D29" s="96">
         <v>0.0</v>
@@ -3438,14 +3443,14 @@
       </c>
       <c r="B30" s="95"/>
       <c r="C30" s="96">
-        <v>152565.0</v>
+        <v>365056.0</v>
       </c>
       <c r="D30" s="96">
-        <v>188.0</v>
+        <v>1404.0</v>
       </c>
       <c r="E30" s="98">
         <f t="shared" si="1"/>
-        <v>0.001232261659</v>
+        <v>0.003845985273</v>
       </c>
       <c r="F30" s="95"/>
     </row>
@@ -3455,14 +3460,14 @@
       </c>
       <c r="B31" s="95"/>
       <c r="C31" s="96">
-        <v>852822.0</v>
+        <v>320082.0</v>
       </c>
       <c r="D31" s="96">
-        <v>338231.0</v>
+        <v>0.0</v>
       </c>
       <c r="E31" s="98">
         <f t="shared" si="1"/>
-        <v>0.3966021045</v>
+        <v>0</v>
       </c>
       <c r="F31" s="95"/>
     </row>
@@ -3472,14 +3477,14 @@
       </c>
       <c r="B32" s="95"/>
       <c r="C32" s="96">
-        <v>328618.0</v>
+        <v>289943.0</v>
       </c>
       <c r="D32" s="96">
-        <v>2607.0</v>
+        <v>18524.0</v>
       </c>
       <c r="E32" s="98">
         <f t="shared" si="1"/>
-        <v>0.007933223378</v>
+        <v>0.06388841945</v>
       </c>
       <c r="F32" s="95"/>
     </row>
@@ -3506,14 +3511,14 @@
       </c>
       <c r="B34" s="95"/>
       <c r="C34" s="96">
-        <v>1004515.0</v>
+        <v>152565.0</v>
       </c>
       <c r="D34" s="96">
-        <v>20983.0</v>
+        <v>188.0</v>
       </c>
       <c r="E34" s="98">
         <f t="shared" si="1"/>
-        <v>0.02088868758</v>
+        <v>0.001232261659</v>
       </c>
       <c r="F34" s="95"/>
     </row>
@@ -3581,16 +3586,24 @@
       </c>
     </row>
     <row r="4" ht="15.75" customHeight="1">
-      <c r="A4" s="103"/>
-      <c r="B4" s="101"/>
-      <c r="C4" s="104"/>
-      <c r="D4" s="101"/>
+      <c r="A4" s="100">
+        <v>44351.0</v>
+      </c>
+      <c r="B4" s="101" t="s">
+        <v>159</v>
+      </c>
+      <c r="C4" s="103">
+        <v>2020.0</v>
+      </c>
+      <c r="D4" s="101" t="s">
+        <v>160</v>
+      </c>
     </row>
     <row r="5" ht="15.75" customHeight="1">
       <c r="A5" s="100"/>
-      <c r="B5" s="105"/>
-      <c r="C5" s="106"/>
-      <c r="D5" s="107"/>
+      <c r="B5" s="104"/>
+      <c r="C5" s="105"/>
+      <c r="D5" s="106"/>
     </row>
   </sheetData>
   <drawing r:id="rId1"/>

</xml_diff>